<commit_message>
Solve multi-window positioning issue
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Missions" sheetId="1" state="visible" r:id="rId3"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="238">
   <si>
     <t xml:space="preserve">GENERAL CONFIGURATION</t>
   </si>
@@ -64,6 +64,9 @@
     <t xml:space="preserve">TrackingSceneResolution [pix]</t>
   </si>
   <si>
+    <t xml:space="preserve">TrackingViewResolution [pix]</t>
+  </si>
+  <si>
     <t xml:space="preserve">MISSION00</t>
   </si>
   <si>
@@ -88,6 +91,9 @@
     <t xml:space="preserve">(20.0, 250.0)</t>
   </si>
   <si>
+    <t xml:space="preserve">(1280x720)</t>
+  </si>
+  <si>
     <t xml:space="preserve">(640x480)</t>
   </si>
   <si>
@@ -719,9 +725,6 @@
   </si>
   <si>
     <t xml:space="preserve">Depth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1280x720)</t>
   </si>
   <si>
     <t xml:space="preserve">CAM06</t>
@@ -1519,10 +1522,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1532,8 +1535,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="54.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="2" width="26.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="37.3"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="11" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="2" width="37.3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="12" style="2" width="11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1549,6 +1552,7 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -1581,111 +1585,126 @@
       <c r="J2" s="6" t="s">
         <v>10</v>
       </c>
+      <c r="K2" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="8"/>
       <c r="B3" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="K4" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>24</v>
-      </c>
       <c r="J5" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="15"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1723,8 +1742,8 @@
   </sheetPr>
   <dimension ref="A1:XFD24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1741,7 +1760,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -1755,48 +1774,48 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E3" s="26" t="n">
         <v>1</v>
@@ -1819,16 +1838,16 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B4" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>219</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>217</v>
-      </c>
       <c r="D4" s="26" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E4" s="26" t="n">
         <v>10</v>
@@ -1851,16 +1870,16 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="26" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E5" s="26" t="n">
         <v>30</v>
@@ -1883,16 +1902,16 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="26" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E6" s="26" t="n">
         <v>15</v>
@@ -1915,16 +1934,16 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="26" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E7" s="26" t="n">
         <v>14</v>
@@ -1947,16 +1966,16 @@
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="26" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>230</v>
+        <v>20</v>
       </c>
       <c r="E8" s="26" t="n">
         <v>10.27</v>
@@ -1979,16 +1998,16 @@
     </row>
     <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="26" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>230</v>
+        <v>20</v>
       </c>
       <c r="E9" s="26" t="n">
         <v>5.5</v>
@@ -2011,16 +2030,16 @@
     </row>
     <row r="10" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="26" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E10" s="26" t="n">
         <v>10</v>
@@ -2029,7 +2048,7 @@
         <v>13.2</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H10" s="26" t="n">
         <v>0.8</v>
@@ -18479,30 +18498,30 @@
         <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D3" s="9" t="n">
         <v>0.5</v>
@@ -18518,13 +18537,13 @@
     </row>
     <row r="4" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>37</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>35</v>
       </c>
       <c r="D4" s="9" t="n">
         <v>1</v>
@@ -18540,13 +18559,13 @@
     </row>
     <row r="5" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D5" s="9" t="n">
         <v>1</v>
@@ -18639,45 +18658,45 @@
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -18727,71 +18746,71 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E3" s="19" t="n">
         <v>16</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E4" s="19" t="n">
         <v>16</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -18842,7 +18861,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -18857,64 +18876,64 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I3" s="23" t="n">
         <v>4</v>
@@ -18928,28 +18947,28 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="23" t="s">
         <v>87</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G4" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>85</v>
       </c>
       <c r="I4" s="23" t="n">
         <v>4</v>
@@ -18963,28 +18982,28 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I5" s="23" t="n">
         <v>4</v>
@@ -18998,28 +19017,28 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I6" s="23" t="n">
         <v>4</v>
@@ -19033,28 +19052,28 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>98</v>
-      </c>
       <c r="F7" s="23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I7" s="23" t="n">
         <v>3</v>
@@ -19068,28 +19087,28 @@
     </row>
     <row r="8" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I8" s="23" t="n">
         <v>3</v>
@@ -19160,7 +19179,7 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -19176,69 +19195,69 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="L2" s="22" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J3" s="23" t="n">
         <v>2</v>
@@ -19252,31 +19271,31 @@
     </row>
     <row r="4" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J4" s="23" t="n">
         <v>10</v>
@@ -19290,31 +19309,31 @@
     </row>
     <row r="5" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J5" s="23" t="n">
         <v>10</v>
@@ -19328,31 +19347,31 @@
     </row>
     <row r="6" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J6" s="23" t="n">
         <v>10</v>
@@ -19366,31 +19385,31 @@
     </row>
     <row r="7" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J7" s="23" t="n">
         <v>2</v>
@@ -19404,31 +19423,31 @@
     </row>
     <row r="8" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J8" s="23" t="n">
         <v>10</v>
@@ -19442,31 +19461,31 @@
     </row>
     <row r="9" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="23" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H9" s="23" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J9" s="23" t="n">
         <v>2</v>
@@ -19480,31 +19499,31 @@
     </row>
     <row r="10" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="23" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J10" s="23" t="n">
         <v>2</v>
@@ -19518,31 +19537,31 @@
     </row>
     <row r="11" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="23" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H11" s="23" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J11" s="23" t="n">
         <v>2</v>
@@ -19556,31 +19575,31 @@
     </row>
     <row r="12" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H12" s="23" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="I12" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J12" s="23" t="n">
         <v>10</v>
@@ -19594,31 +19613,31 @@
     </row>
     <row r="13" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="23" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H13" s="23" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J13" s="23" t="n">
         <v>10</v>
@@ -19632,31 +19651,31 @@
     </row>
     <row r="14" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="23" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H14" s="23" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="I14" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J14" s="23" t="n">
         <v>10</v>
@@ -19670,31 +19689,31 @@
     </row>
     <row r="15" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H15" s="23" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I15" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J15" s="23" t="n">
         <v>10</v>
@@ -19708,31 +19727,31 @@
     </row>
     <row r="16" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H16" s="23" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I16" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J16" s="23" t="n">
         <v>30</v>
@@ -19800,7 +19819,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -19814,45 +19833,45 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D3" s="26" t="n">
         <v>10</v>
@@ -19878,13 +19897,13 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D4" s="26" t="n">
         <v>8</v>
@@ -19960,7 +19979,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -19971,39 +19990,39 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E3" s="26" t="n">
         <v>0.4</v>
@@ -20017,16 +20036,16 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C4" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" s="26" t="s">
         <v>189</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>187</v>
       </c>
       <c r="E4" s="26" t="n">
         <v>0.6</v>
@@ -20087,7 +20106,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -20101,57 +20120,57 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C3" s="26" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F3" s="26" t="n">
         <v>50</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="H3" s="26" t="n">
         <v>270</v>
@@ -20165,25 +20184,25 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C4" s="26" t="n">
         <v>2</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F4" s="26" t="n">
         <v>50</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="H4" s="26" t="n">
         <v>180</v>
@@ -20197,25 +20216,25 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="26" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C5" s="26" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F5" s="26" t="n">
         <v>50</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="H5" s="26" t="n">
         <v>270</v>
@@ -20229,25 +20248,25 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="26" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C6" s="26" t="n">
         <v>2</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F6" s="26" t="n">
         <v>50</v>
       </c>
       <c r="G6" s="26" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="H6" s="26" t="n">
         <v>180</v>
@@ -20261,25 +20280,25 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="26" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C7" s="26" t="n">
         <v>3</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F7" s="26" t="n">
         <v>50</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="H7" s="26" t="n">
         <v>180</v>

</xml_diff>

<commit_message>
Solve projection issues and add window drawing
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Missions" sheetId="1" state="visible" r:id="rId3"/>
@@ -2104,7 +2104,7 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -2810,8 +2810,8 @@
   </sheetPr>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Upgrade positioning by adjusting weights
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Missions" sheetId="1" state="visible" r:id="rId3"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="241">
   <si>
     <t xml:space="preserve">GENERAL CONFIGURATION</t>
   </si>
@@ -91,648 +91,651 @@
     <t xml:space="preserve">(20.0, 250.0)</t>
   </si>
   <si>
+    <t xml:space="preserve">(854x480)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(640x360)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MISSION01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single-Agent Multi-Camera Wreck Rescue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUNDLE01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEAM01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(35.0, 280.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MISSION02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single-Agent Multi-Window Wreck Rescue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEAM02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SimulationName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autopilot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClockSpeed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RecordMetrics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DrawRvizMarkers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DrawWorldMarkers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slow Simple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SimpleFlight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIM01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regular Simple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIM02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regular PX4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PX4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MapName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RegionType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OriginGeopoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StartDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StartHour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WindVelocity [m/s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ocean Coast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coastal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(lat=47.64, lon=-122.14, alt=122.00)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(13/12/2024)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(20:00:00)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Vx=0.0, Vy=0.0, Vz=0.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GroupID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GroupName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TargetType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TargetCount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GroupPriority</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TrajectoryFolder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GROUP00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fast Human Targets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HighSpeed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GROUP01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slow Human Targets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LowSpeed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGENT CONFIGURATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgentID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AgentName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HeadPayloadID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TrackingMode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DroneModelID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InitialPosition [m]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InitialOrientation [°]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SafetyRadius [m]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxAltitude [m]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BatteryCapacity [mAh]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGENT00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAYLOAD00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MultiWindowTracking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DRONE00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=15.0, Y=20.0, Z=50.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Pitch=0.0, Yaw=0.0, Roll=0.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGENT01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAYLOAD01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=10.0, Y=-20.0, Z=40.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGENT02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAYLOAD02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PriorityHybridTracking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=-25.0, Y=10.0, Z=70.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGENT03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAYLOAD03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MultiCameraTracking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=-15.0, Y=-20.0, Z=30.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGENT04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAYLOAD04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=-35.0, Y=-20.0, Z=25.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGENT05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAYLOAD05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=15.0, Y=20.0, Z=100.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HeadID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HeadName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GimbalModelID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CameraModelID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HeadRole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MountPosition [m]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MountOrientation [°]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InitialFocal [mm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MinFocal [mm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxFocal [mm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.1 Central Cam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIMBAL00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAM00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=0.0, Y=0.0, Z=-0.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Pitch=90, Yaw=90, Roll=0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.1 Tracking Cam 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIMBAL01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAM01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tracking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=0.3, Y=0.0, Z=-0.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Pitch=90, Yaw=0, Roll=0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.1 Tracking Cam 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=0.0, Y=0.3, Z=-0.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.1 Tracking Cam 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=-0.3, Y=0.0, Z=-0.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Pitch=90, Yaw=180, Roll=0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.2 Central Cam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.2 Tracking Cam 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.3 Central Cam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 1.4 Central Cam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 2.1 Central Cam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Pitch=0, Yaw=90, Roll=0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 2.1 Tracking Cam 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Pitch=0, Yaw=0, Roll=0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 2.1 Tracking Cam 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 2.1 Tracking Cam 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Pitch=0, Yaw=180, Roll=0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 2.1 Tracking Cam 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=0.0, Y=-0.3, Z=-0.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Pitch=0, Yaw=270, Roll=0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent 3.1 Central Cam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAM07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HARDWARE CATALOGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DroneName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DroneType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CruiseSpeed [m/s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxSpeed [m/s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BaseWeight [kg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxPayloadWeight [kg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HoverPower [W]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CruisePower [W]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LoadFactor [W/kg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default Quadcopter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quadcopter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DRONE01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default Hexacopter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hexacopter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GimbalName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LinkConfigurationID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpticalCenterOffset [mm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weight [kg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IdlePower [W]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ActivePower [W]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default Central Gimbal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINKCONFIG00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=0.0, Y=0.0, Z=0.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default Tracking Gimbal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINKCONFIG01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GimbalLinkID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LinkIndex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AxisType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LinkOffset [mm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LinkLength [mm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JointRange [°]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxAngularSpeed [°/s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MotorRiseTime [s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MotorDampingFactor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINK00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-320.0, 320.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINK01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pitch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-40.0, 130.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINK02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINK03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-20.0, 20.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINK04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CameraName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CameraType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resolution [pix]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DefaultFocal [mm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SensorWidth [mm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SensorHeight [mm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raspberry Pi Camera HQ Lens 2.8 12mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2560x1440)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mavic 2 Pro (Mod. Zoom)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1920x1080)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAM02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zenmuse P1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAM03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zenmuse X5S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAM04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raspberry Pi Camera HQ Lens 6 22mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAM05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mavic 2 Pro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depth</t>
+  </si>
+  <si>
     <t xml:space="preserve">(1280x720)</t>
   </si>
   <si>
-    <t xml:space="preserve">(640x480)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MISSION01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Single-Agent Multi-Camera Wreck Rescue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUNDLE01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEAM01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(35.0, 280.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MISSION02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Single-Agent Multi-Window Wreck Rescue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEAM02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SimulationName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Autopilot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClockSpeed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RecordMetrics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DrawRvizMarkers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DrawWorldMarkers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slow Simple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SimpleFlight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIM01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regular Simple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIM02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regular PX4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PX4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MapName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RegionType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OriginGeopoint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StartDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StartHour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WindVelocity [m/s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ocean Coast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coastal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(lat=47.64, lon=-122.14, alt=122.00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(13/12/2024)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(20:00:00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Vx=0.0, Vy=0.0, Vz=0.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GroupID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GroupName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TargetType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TargetCount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GroupPriority</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TrajectoryFolder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GROUP00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fast Human Targets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Human</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HighSpeed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GROUP01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slow Human Targets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LowSpeed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGENT CONFIGURATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AgentID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AgentName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HeadPayloadID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TrackingMode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DroneModelID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InitialPosition [m]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InitialOrientation [°]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SafetyRadius [m]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxAltitude [m]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BatteryCapacity [mAh]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGENT00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAYLOAD00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MultiWindowTracking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DRONE00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=15.0, Y=20.0, Z=50.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Pitch=0.0, Yaw=0.0, Roll=0.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGENT01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAYLOAD01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=10.0, Y=-20.0, Z=40.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGENT02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAYLOAD02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PriorityHybridTracking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=-25.0, Y=10.0, Z=70.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGENT03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAYLOAD03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MultiCameraTracking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=-15.0, Y=-20.0, Z=30.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGENT04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAYLOAD04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=-35.0, Y=-20.0, Z=25.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGENT05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 3.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAYLOAD05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=15.0, Y=20.0, Z=100.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HeadID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HeadName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GimbalModelID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CameraModelID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HeadRole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MountPosition [m]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MountOrientation [°]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InitialFocal [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MinFocal [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxFocal [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.1 Central Cam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIMBAL00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAM00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=0.0, Y=0.0, Z=-0.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Pitch=90, Yaw=90, Roll=0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.1 Tracking Cam 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIMBAL01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAM01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tracking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=0.3, Y=0.0, Z=-0.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Pitch=90, Yaw=0, Roll=0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.1 Tracking Cam 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=0.0, Y=0.3, Z=-0.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.1 Tracking Cam 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=-0.3, Y=0.0, Z=-0.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Pitch=90, Yaw=180, Roll=0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.2 Central Cam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.2 Tracking Cam 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.3 Central Cam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 1.4 Central Cam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 2.1 Central Cam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Pitch=0, Yaw=90, Roll=0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 2.1 Tracking Cam 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Pitch=0, Yaw=0, Roll=0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 2.1 Tracking Cam 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 2.1 Tracking Cam 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Pitch=0, Yaw=180, Roll=0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 2.1 Tracking Cam 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=0.0, Y=-0.3, Z=-0.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Pitch=0, Yaw=270, Roll=0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agent 3.1 Central Cam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAM07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HARDWARE CATALOGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DroneName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DroneType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CruiseSpeed [m/s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxSpeed [m/s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BaseWeight [kg]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxPayloadWeight [kg]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HoverPower [W]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CruisePower [W]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LoadFactor [W/kg]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default Quadcopter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quadcopter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DRONE01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default Hexacopter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hexacopter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GimbalName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LinkConfigurationID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OpticalCenterOffset [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weight [kg]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IdlePower [W]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ActivePower [W]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default Central Gimbal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINKCONFIG00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=0.0, Y=0.0, Z=0.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default Tracking Gimbal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINKCONFIG01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GimbalLinkID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LinkIndex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AxisType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LinkOffset [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LinkLength [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JointRange [°]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxAngularSpeed [°/s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MotorRiseTime [s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MotorDampingFactor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINK00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yaw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-320.0, 320.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINK01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pitch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-40.0, 130.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINK02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINK03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-20.0, 20.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINK04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CameraName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CameraType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resolution [pix]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DefaultFocal [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SensorWidth [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SensorHeight [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raspberry Pi Camera HQ Lens 2.8 12mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RGB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2560x1440)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mavic 2 Pro (Mod. Zoom)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1920x1080)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAM02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zenmuse P1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAM03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zenmuse X5S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAM04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raspberry Pi Camera HQ Lens 6 22mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAM05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mavic 2 Pro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depth</t>
-  </si>
-  <si>
     <t xml:space="preserve">CAM06</t>
   </si>
   <si>
@@ -745,7 +748,7 @@
     <t xml:space="preserve">Zenmuse X9-8K</t>
   </si>
   <si>
-    <t xml:space="preserve">(8192x5456)</t>
+    <t xml:space="preserve">(8192x4608)</t>
   </si>
   <si>
     <t xml:space="preserve">8.8</t>
@@ -1748,8 +1751,8 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1981,7 +1984,7 @@
         <v>233</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>20</v>
+        <v>234</v>
       </c>
       <c r="E8" s="26" t="n">
         <v>10.27</v>
@@ -2004,16 +2007,16 @@
     </row>
     <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>237</v>
+      </c>
+      <c r="D9" s="26" t="s">
         <v>234</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>235</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>20</v>
       </c>
       <c r="E9" s="26" t="n">
         <v>5.5</v>
@@ -2039,13 +2042,13 @@
         <v>167</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>221</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E10" s="26" t="n">
         <v>3.5</v>
@@ -2054,7 +2057,7 @@
         <v>13.2</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="H10" s="26" t="n">
         <v>0.8</v>
@@ -2810,7 +2813,7 @@
   </sheetPr>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Prepare project to link with PX4 Autopilot and MAVROS
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Missions" sheetId="1" state="visible" r:id="rId3"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="240">
   <si>
     <t xml:space="preserve">GENERAL CONFIGURATION</t>
   </si>
@@ -121,6 +121,9 @@
     <t xml:space="preserve">Single-Agent Multi-Window Wreck Rescue</t>
   </si>
   <si>
+    <t xml:space="preserve">SIM02</t>
+  </si>
+  <si>
     <t xml:space="preserve">TEAM02</t>
   </si>
   <si>
@@ -154,15 +157,15 @@
     <t xml:space="preserve">Regular Simple</t>
   </si>
   <si>
-    <t xml:space="preserve">SIM02</t>
-  </si>
-  <si>
     <t xml:space="preserve">Regular PX4</t>
   </si>
   <si>
     <t xml:space="preserve">PX4</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t xml:space="preserve">MapName</t>
   </si>
   <si>
@@ -746,9 +749,6 @@
   </si>
   <si>
     <t xml:space="preserve">Zenmuse X9-8K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(8192x4608)</t>
   </si>
 </sst>
 </file>
@@ -761,7 +761,7 @@
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -829,6 +829,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -924,7 +930,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -973,6 +979,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -985,7 +995,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1530,8 +1540,8 @@
   </sheetPr>
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1661,7 +1671,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" s="13" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
         <v>27</v>
       </c>
@@ -1671,8 +1681,8 @@
       <c r="C5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>14</v>
+      <c r="D5" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>15</v>
@@ -1684,7 +1694,7 @@
         <v>17</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>26</v>
@@ -1697,20 +1707,20 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="15"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
+      <c r="B8" s="16"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
     </row>
     <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1748,8 +1758,8 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1757,7 +1767,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="39.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="20" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="21" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="2" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="30.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="26.66"/>
@@ -1765,304 +1775,304 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+    </row>
+    <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="E3" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="27" t="n">
+        <v>6.287</v>
+      </c>
+      <c r="G3" s="27" t="n">
+        <v>4.712</v>
+      </c>
+      <c r="H3" s="27" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I3" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="J3" s="27" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="E4" s="27" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" s="27" t="n">
+        <v>13.2</v>
+      </c>
+      <c r="G4" s="27" t="n">
+        <v>8.8</v>
+      </c>
+      <c r="H4" s="27" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I4" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="J4" s="27" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="E5" s="27" t="n">
+        <v>30</v>
+      </c>
+      <c r="F5" s="27" t="n">
+        <v>35.9</v>
+      </c>
+      <c r="G5" s="27" t="n">
+        <v>24</v>
+      </c>
+      <c r="H5" s="27" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I5" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="J5" s="27" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="E6" s="27" t="n">
+        <v>15</v>
+      </c>
+      <c r="F6" s="27" t="n">
+        <v>17.3</v>
+      </c>
+      <c r="G6" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="H6" s="27" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I6" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" s="27" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="E7" s="27" t="n">
+        <v>14</v>
+      </c>
+      <c r="F7" s="27" t="n">
+        <v>6.287</v>
+      </c>
+      <c r="G7" s="27" t="n">
+        <v>4.712</v>
+      </c>
+      <c r="H7" s="27" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I7" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" s="27" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="E8" s="27" t="n">
+        <v>10.27</v>
+      </c>
+      <c r="F8" s="27" t="n">
+        <v>13.2</v>
+      </c>
+      <c r="G8" s="27" t="n">
+        <v>8.8</v>
+      </c>
+      <c r="H8" s="27" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="27" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="E9" s="27" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="F9" s="27" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="G9" s="28" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="H9" s="27" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="I9" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="J9" s="27" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" s="13" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-    </row>
-    <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
-        <v>114</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>214</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>215</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>216</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>217</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>218</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>219</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>186</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>220</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>221</v>
-      </c>
-      <c r="D3" s="26" t="s">
+      <c r="B10" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="C10" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="E3" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="26" t="n">
-        <v>6.287</v>
-      </c>
-      <c r="G3" s="26" t="n">
-        <v>4.712</v>
-      </c>
-      <c r="H3" s="26" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="I3" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="J3" s="26" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" s="26" t="s">
+      <c r="D10" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>221</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="E4" s="26" t="n">
-        <v>10</v>
-      </c>
-      <c r="F4" s="26" t="n">
+      <c r="E10" s="27" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="F10" s="27" t="n">
         <v>13.2</v>
       </c>
-      <c r="G4" s="26" t="n">
-        <v>8.8</v>
-      </c>
-      <c r="H4" s="26" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I4" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="J4" s="26" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="26" t="s">
-        <v>225</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>226</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>221</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="E5" s="26" t="n">
-        <v>30</v>
-      </c>
-      <c r="F5" s="26" t="n">
-        <v>35.9</v>
-      </c>
-      <c r="G5" s="26" t="n">
-        <v>24</v>
-      </c>
-      <c r="H5" s="26" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="I5" s="26" t="n">
+      <c r="G10" s="27" t="n">
+        <v>7.425</v>
+      </c>
+      <c r="H10" s="27" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="I10" s="27" t="n">
         <v>3</v>
       </c>
-      <c r="J5" s="26" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="26" t="s">
-        <v>227</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>221</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="E6" s="26" t="n">
-        <v>15</v>
-      </c>
-      <c r="F6" s="26" t="n">
-        <v>17.3</v>
-      </c>
-      <c r="G6" s="26" t="n">
-        <v>13</v>
-      </c>
-      <c r="H6" s="26" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I6" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="J6" s="26" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>230</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>221</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="E7" s="26" t="n">
-        <v>14</v>
-      </c>
-      <c r="F7" s="26" t="n">
-        <v>6.287</v>
-      </c>
-      <c r="G7" s="26" t="n">
-        <v>4.712</v>
-      </c>
-      <c r="H7" s="26" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="I7" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="J7" s="26" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="26" t="s">
-        <v>231</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>232</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>233</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>234</v>
-      </c>
-      <c r="E8" s="26" t="n">
-        <v>10.27</v>
-      </c>
-      <c r="F8" s="26" t="n">
-        <v>13.2</v>
-      </c>
-      <c r="G8" s="26" t="n">
-        <v>8.8</v>
-      </c>
-      <c r="H8" s="26" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I8" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" s="26" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="26" t="s">
-        <v>235</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>237</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>234</v>
-      </c>
-      <c r="E9" s="26" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="F9" s="26" t="n">
-        <v>6.3</v>
-      </c>
-      <c r="G9" s="27" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="H9" s="26" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="I9" s="26" t="n">
-        <v>3</v>
-      </c>
-      <c r="J9" s="26" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>221</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>239</v>
-      </c>
-      <c r="E10" s="26" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="F10" s="26" t="n">
-        <v>13.2</v>
-      </c>
-      <c r="G10" s="26" t="n">
-        <v>7.425</v>
-      </c>
-      <c r="H10" s="26" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="I10" s="26" t="n">
-        <v>3</v>
-      </c>
-      <c r="J10" s="26" t="n">
+      <c r="J10" s="27" t="n">
         <v>6</v>
       </c>
     </row>
@@ -2105,7 +2115,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2116,37 +2126,37 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2154,15 +2164,15 @@
         <v>14</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D3" s="9" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="E3" s="17" t="b">
+        <v>0.1</v>
+      </c>
+      <c r="E3" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2177,33 +2187,33 @@
     </row>
     <row r="4" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>38</v>
       </c>
       <c r="D4" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="17" t="b">
+      <c r="E4" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F4" s="17" t="b">
+      <c r="F4" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G4" s="17" t="b">
+      <c r="G4" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>42</v>
@@ -2212,37 +2222,39 @@
         <v>43</v>
       </c>
       <c r="D5" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="17" t="b">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F5" s="17" t="b">
+      <c r="F5" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G5" s="17" t="b">
+      <c r="G5" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C6" s="14"/>
+      <c r="C6" s="15"/>
     </row>
     <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C7" s="14"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
     </row>
     <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
+      <c r="A9" s="16"/>
+      <c r="D9" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2291,37 +2303,37 @@
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2329,22 +2341,22 @@
         <v>15</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G3" s="18" t="s">
         <v>55</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2382,83 +2394,83 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="19" t="n">
+        <v>65</v>
+      </c>
+      <c r="E3" s="20" t="n">
         <v>16</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="19" t="n">
+        <v>65</v>
+      </c>
+      <c r="E4" s="20" t="n">
         <v>16</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2499,7 +2511,7 @@
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="20" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="21" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="29.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="32.44"/>
@@ -2508,263 +2520,263 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
+      <c r="A1" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="22" t="s">
+      <c r="A2" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" s="22" t="s">
+      <c r="C2" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="D2" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="E2" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="F2" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="G2" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="H2" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="I2" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="J2" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="M2" s="12"/>
+      <c r="K2" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="M2" s="13"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="23" t="s">
+      <c r="A3" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" s="23" t="s">
+      <c r="C3" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="D3" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="E3" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="F3" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="G3" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="I3" s="23" t="n">
+      <c r="H3" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="24" t="n">
         <v>4</v>
       </c>
-      <c r="J3" s="23" t="n">
+      <c r="J3" s="24" t="n">
         <v>250</v>
       </c>
-      <c r="K3" s="23" t="n">
+      <c r="K3" s="24" t="n">
         <v>10000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="I4" s="24" t="n">
+        <v>4</v>
+      </c>
+      <c r="J4" s="24" t="n">
+        <v>250</v>
+      </c>
+      <c r="K4" s="24" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="F4" s="23" t="s">
+      <c r="C5" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="I5" s="24" t="n">
+        <v>4</v>
+      </c>
+      <c r="J5" s="24" t="n">
+        <v>250</v>
+      </c>
+      <c r="K5" s="24" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="I6" s="24" t="n">
+        <v>4</v>
+      </c>
+      <c r="J6" s="24" t="n">
+        <v>250</v>
+      </c>
+      <c r="K6" s="24" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="24" t="n">
+        <v>3</v>
+      </c>
+      <c r="J7" s="24" t="n">
+        <v>300</v>
+      </c>
+      <c r="K7" s="24" t="n">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="8" s="13" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="G4" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="I4" s="23" t="n">
-        <v>4</v>
-      </c>
-      <c r="J4" s="23" t="n">
-        <v>250</v>
-      </c>
-      <c r="K4" s="23" t="n">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="I5" s="23" t="n">
-        <v>4</v>
-      </c>
-      <c r="J5" s="23" t="n">
-        <v>250</v>
-      </c>
-      <c r="K5" s="23" t="n">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="I6" s="23" t="n">
-        <v>4</v>
-      </c>
-      <c r="J6" s="23" t="n">
-        <v>250</v>
-      </c>
-      <c r="K6" s="23" t="n">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="I7" s="23" t="n">
+      <c r="F8" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" s="24" t="n">
         <v>3</v>
       </c>
-      <c r="J7" s="23" t="n">
+      <c r="J8" s="24" t="n">
         <v>300</v>
       </c>
-      <c r="K7" s="23" t="n">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="8" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="I8" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="J8" s="23" t="n">
-        <v>300</v>
-      </c>
-      <c r="K8" s="23" t="n">
+      <c r="K8" s="24" t="n">
         <v>12000</v>
       </c>
       <c r="L8" s="2"/>
@@ -2817,7 +2829,7 @@
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="2" width="27.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="20" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="21" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="2" width="27.34"/>
@@ -2825,588 +2837,588 @@
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
+      <c r="A1" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="22" t="s">
+      <c r="A2" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="B2" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="D2" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="E2" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="F2" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="G2" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="I2" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="J2" s="22" t="s">
+      <c r="H2" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="I2" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="K2" s="23" t="s">
         <v>120</v>
       </c>
+      <c r="L2" s="23" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="3" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="23" t="s">
+      <c r="A3" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="B3" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="D3" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="E3" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="F3" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="G3" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="I3" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="J3" s="23" t="n">
+      <c r="H3" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="K3" s="23" t="n">
+      <c r="K3" s="24" t="n">
         <v>0.5</v>
       </c>
-      <c r="L3" s="23" t="n">
+      <c r="L3" s="24" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="J4" s="24" t="n">
+        <v>10</v>
+      </c>
+      <c r="K4" s="24" t="n">
+        <v>8</v>
+      </c>
+      <c r="L4" s="24" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H5" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="E4" s="23" t="s">
+      <c r="I5" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="J5" s="24" t="n">
+        <v>10</v>
+      </c>
+      <c r="K5" s="24" t="n">
+        <v>8</v>
+      </c>
+      <c r="L5" s="24" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="E6" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="F6" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="G6" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="I6" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="J6" s="24" t="n">
+        <v>10</v>
+      </c>
+      <c r="K6" s="24" t="n">
+        <v>8</v>
+      </c>
+      <c r="L6" s="24" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="J7" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" s="24" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L7" s="24" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="G8" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="I4" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="J4" s="23" t="n">
+      <c r="H8" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="J8" s="24" t="n">
         <v>10</v>
       </c>
-      <c r="K4" s="23" t="n">
+      <c r="K8" s="24" t="n">
         <v>8</v>
       </c>
-      <c r="L4" s="23" t="n">
+      <c r="L8" s="24" t="n">
         <v>40</v>
       </c>
     </row>
-    <row r="5" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="E5" s="23" t="s">
+    <row r="9" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="J9" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="K9" s="24" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L9" s="24" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="J10" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" s="24" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L10" s="24" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="I11" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="J11" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="K11" s="24" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L11" s="24" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="D12" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="E12" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="G5" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="H5" s="23" t="s">
+      <c r="F12" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="I12" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="J12" s="24" t="n">
+        <v>10</v>
+      </c>
+      <c r="K12" s="24" t="n">
+        <v>8</v>
+      </c>
+      <c r="L12" s="24" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="I13" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="J13" s="24" t="n">
+        <v>10</v>
+      </c>
+      <c r="K13" s="24" t="n">
+        <v>8</v>
+      </c>
+      <c r="L13" s="24" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="I14" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="J14" s="24" t="n">
+        <v>10</v>
+      </c>
+      <c r="K14" s="24" t="n">
+        <v>8</v>
+      </c>
+      <c r="L14" s="24" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="J15" s="24" t="n">
+        <v>10</v>
+      </c>
+      <c r="K15" s="24" t="n">
+        <v>8</v>
+      </c>
+      <c r="L15" s="24" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" s="13" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="G16" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="I5" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="J5" s="23" t="n">
-        <v>10</v>
-      </c>
-      <c r="K5" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="L5" s="23" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="I6" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="J6" s="23" t="n">
-        <v>10</v>
-      </c>
-      <c r="K6" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="L6" s="23" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="I7" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="J7" s="23" t="n">
+      <c r="H16" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="J16" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="K7" s="23" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L7" s="23" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="I8" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="J8" s="23" t="n">
-        <v>10</v>
-      </c>
-      <c r="K8" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="L8" s="23" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="I9" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="J9" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="K9" s="23" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L9" s="23" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="F10" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="G10" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="H10" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="I10" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="J10" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="K10" s="23" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L10" s="23" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="H11" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="J11" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="K11" s="23" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L11" s="23" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="H12" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="I12" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="J12" s="23" t="n">
-        <v>10</v>
-      </c>
-      <c r="K12" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="L12" s="23" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>157</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="H13" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="I13" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="J13" s="23" t="n">
-        <v>10</v>
-      </c>
-      <c r="K13" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="L13" s="23" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="H14" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="J14" s="23" t="n">
-        <v>10</v>
-      </c>
-      <c r="K14" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="L14" s="23" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="23" t="s">
-        <v>161</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="H15" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="I15" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="J15" s="23" t="n">
-        <v>10</v>
-      </c>
-      <c r="K15" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="L15" s="23" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="F16" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="H16" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="I16" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="J16" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="K16" s="23" t="n">
+      <c r="K16" s="24" t="n">
         <v>0.1</v>
       </c>
-      <c r="L16" s="23" t="n">
+      <c r="L16" s="24" t="n">
         <v>12</v>
       </c>
       <c r="M16" s="2"/>
@@ -3452,125 +3464,125 @@
   </sheetPr>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="20" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="21" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="2" width="26.66"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="11" style="2" width="11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="A1" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>169</v>
-      </c>
-      <c r="C2" s="25" t="s">
+      <c r="A2" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="C2" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="D2" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="E2" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="F2" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="G2" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="H2" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="I2" s="26" t="s">
         <v>177</v>
       </c>
+      <c r="J2" s="26" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>178</v>
-      </c>
-      <c r="C3" s="26" t="s">
+      <c r="A3" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="D3" s="26" t="n">
+      <c r="C3" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="D3" s="27" t="n">
         <v>10</v>
       </c>
-      <c r="E3" s="26" t="n">
+      <c r="E3" s="27" t="n">
         <v>15</v>
       </c>
-      <c r="F3" s="26" t="n">
+      <c r="F3" s="27" t="n">
         <v>4.5</v>
       </c>
-      <c r="G3" s="26" t="n">
+      <c r="G3" s="27" t="n">
         <v>1.5</v>
       </c>
-      <c r="H3" s="26" t="n">
+      <c r="H3" s="27" t="n">
         <v>250</v>
       </c>
-      <c r="I3" s="26" t="n">
+      <c r="I3" s="27" t="n">
         <v>200</v>
       </c>
-      <c r="J3" s="26" t="n">
+      <c r="J3" s="27" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="s">
-        <v>180</v>
-      </c>
-      <c r="B4" s="26" t="s">
+      <c r="A4" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="D4" s="26" t="n">
+      <c r="C4" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" s="27" t="n">
         <v>8</v>
       </c>
-      <c r="E4" s="26" t="n">
+      <c r="E4" s="27" t="n">
         <v>12</v>
       </c>
-      <c r="F4" s="26" t="n">
+      <c r="F4" s="27" t="n">
         <v>6.5</v>
       </c>
-      <c r="G4" s="26" t="n">
+      <c r="G4" s="27" t="n">
         <v>2.5</v>
       </c>
-      <c r="H4" s="26" t="n">
+      <c r="H4" s="27" t="n">
         <v>400</v>
       </c>
-      <c r="I4" s="26" t="n">
+      <c r="I4" s="27" t="n">
         <v>350</v>
       </c>
-      <c r="J4" s="26" t="n">
+      <c r="J4" s="27" t="n">
         <v>25</v>
       </c>
     </row>
@@ -3625,82 +3637,82 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="A1" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="C2" s="25" t="s">
+      <c r="A2" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="C2" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="D2" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="E2" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="F2" s="26" t="s">
         <v>188</v>
       </c>
+      <c r="G2" s="26" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>189</v>
-      </c>
-      <c r="C3" s="26" t="s">
+      <c r="A3" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="C3" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="E3" s="26" t="n">
+      <c r="D3" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" s="27" t="n">
         <v>0.4</v>
       </c>
-      <c r="F3" s="26" t="n">
+      <c r="F3" s="27" t="n">
         <v>5</v>
       </c>
-      <c r="G3" s="26" t="n">
+      <c r="G3" s="27" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="B4" s="26" t="s">
+      <c r="A4" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" s="27" t="s">
         <v>192</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>191</v>
-      </c>
-      <c r="E4" s="26" t="n">
+      <c r="E4" s="27" t="n">
         <v>0.6</v>
       </c>
-      <c r="F4" s="26" t="n">
+      <c r="F4" s="27" t="n">
         <v>10</v>
       </c>
-      <c r="G4" s="26" t="n">
+      <c r="G4" s="27" t="n">
         <v>20</v>
       </c>
     </row>
@@ -3752,208 +3764,208 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="A1" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="F3" s="27" t="n">
+        <v>50</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="H3" s="27" t="n">
+        <v>270</v>
+      </c>
+      <c r="I3" s="27" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="J3" s="27" t="n">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="F4" s="27" t="n">
+        <v>50</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="H4" s="27" t="n">
+        <v>180</v>
+      </c>
+      <c r="I4" s="27" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="J4" s="27" t="n">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="B5" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>198</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>199</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>190</v>
-      </c>
-      <c r="C3" s="26" t="n">
+      <c r="C5" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="26" t="s">
-        <v>204</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>191</v>
-      </c>
-      <c r="F3" s="26" t="n">
+      <c r="D5" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="F5" s="27" t="n">
         <v>50</v>
       </c>
-      <c r="G3" s="26" t="s">
-        <v>205</v>
-      </c>
-      <c r="H3" s="26" t="n">
+      <c r="G5" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="H5" s="27" t="n">
         <v>270</v>
       </c>
-      <c r="I3" s="26" t="n">
+      <c r="I5" s="27" t="n">
         <v>0.06</v>
       </c>
-      <c r="J3" s="26" t="n">
+      <c r="J5" s="27" t="n">
         <v>0.95</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="s">
-        <v>206</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>190</v>
-      </c>
-      <c r="C4" s="26" t="n">
+    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="C6" s="27" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>191</v>
-      </c>
-      <c r="F4" s="26" t="n">
+      <c r="D6" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="F6" s="27" t="n">
         <v>50</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G6" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="H6" s="27" t="n">
+        <v>180</v>
+      </c>
+      <c r="I6" s="27" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J6" s="27" t="n">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" s="27" t="s">
         <v>208</v>
       </c>
-      <c r="H4" s="26" t="n">
+      <c r="E7" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="F7" s="27" t="n">
+        <v>50</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="H7" s="27" t="n">
         <v>180</v>
       </c>
-      <c r="I4" s="26" t="n">
+      <c r="I7" s="27" t="n">
         <v>0.05</v>
       </c>
-      <c r="J4" s="26" t="n">
-        <v>0.97</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="C5" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>204</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>191</v>
-      </c>
-      <c r="F5" s="26" t="n">
-        <v>50</v>
-      </c>
-      <c r="G5" s="26" t="s">
-        <v>205</v>
-      </c>
-      <c r="H5" s="26" t="n">
-        <v>270</v>
-      </c>
-      <c r="I5" s="26" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="J5" s="26" t="n">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="C6" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>211</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>191</v>
-      </c>
-      <c r="F6" s="26" t="n">
-        <v>50</v>
-      </c>
-      <c r="G6" s="26" t="s">
-        <v>212</v>
-      </c>
-      <c r="H6" s="26" t="n">
-        <v>180</v>
-      </c>
-      <c r="I6" s="26" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="J6" s="26" t="n">
-        <v>0.97</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="26" t="s">
-        <v>213</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="C7" s="26" t="n">
-        <v>3</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="E7" s="26" t="s">
-        <v>191</v>
-      </c>
-      <c r="F7" s="26" t="n">
-        <v>50</v>
-      </c>
-      <c r="G7" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="H7" s="26" t="n">
-        <v>180</v>
-      </c>
-      <c r="I7" s="26" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="J7" s="26" t="n">
+      <c r="J7" s="27" t="n">
         <v>0.99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add support for gimbal APIs
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Missions" sheetId="1" state="visible" r:id="rId3"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="236">
   <si>
     <t xml:space="preserve">GENERAL CONFIGURATION</t>
   </si>
@@ -403,7 +403,7 @@
     <t xml:space="preserve">Agent 1.1 Central Cam</t>
   </si>
   <si>
-    <t xml:space="preserve">GIMBAL00</t>
+    <t xml:space="preserve">GIM00</t>
   </si>
   <si>
     <t xml:space="preserve">CAM00</t>
@@ -424,7 +424,7 @@
     <t xml:space="preserve">Agent 1.1 Tracking Cam 1</t>
   </si>
   <si>
-    <t xml:space="preserve">GIMBAL01</t>
+    <t xml:space="preserve">GIM01</t>
   </si>
   <si>
     <t xml:space="preserve">CAM01</t>
@@ -589,9 +589,6 @@
     <t xml:space="preserve">LinkConfigurationID</t>
   </si>
   <si>
-    <t xml:space="preserve">OpticalCenterOffset [mm]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Weight [kg]</t>
   </si>
   <si>
@@ -607,9 +604,6 @@
     <t xml:space="preserve">LINKCONFIG00</t>
   </si>
   <si>
-    <t xml:space="preserve">(X=0.0, Y=0.0, Z=0.0)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Default Tracking Gimbal</t>
   </si>
   <si>
@@ -619,18 +613,9 @@
     <t xml:space="preserve">GimbalLinkID</t>
   </si>
   <si>
-    <t xml:space="preserve">LinkIndex</t>
-  </si>
-  <si>
     <t xml:space="preserve">AxisType</t>
   </si>
   <si>
-    <t xml:space="preserve">LinkOffset [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LinkLength [mm]</t>
-  </si>
-  <si>
     <t xml:space="preserve">JointRange [°]</t>
   </si>
   <si>
@@ -646,31 +631,31 @@
     <t xml:space="preserve">LINK00</t>
   </si>
   <si>
+    <t xml:space="preserve">Roll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-20.0, 20.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINK01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pitch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-40.0, 130.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINK02</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yaw</t>
   </si>
   <si>
     <t xml:space="preserve">(-320.0, 320.0)</t>
   </si>
   <si>
-    <t xml:space="preserve">LINK01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pitch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-40.0, 130.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINK02</t>
-  </si>
-  <si>
     <t xml:space="preserve">LINK03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-20.0, 20.0)</t>
   </si>
   <si>
     <t xml:space="preserve">LINK04</t>
@@ -927,7 +912,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1022,6 +1007,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1222,9 +1211,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table210" displayName="Table210" ref="A2:L15" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A2:L15"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table210" displayName="Table210" ref="A2:K15" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A2:K15"/>
+  <tableColumns count="11">
     <tableColumn id="1" name="HeadID"/>
     <tableColumn id="2" name="HeadPayloadID"/>
     <tableColumn id="3" name="HeadName"/>
@@ -1233,10 +1222,9 @@
     <tableColumn id="6" name="HeadRole"/>
     <tableColumn id="7" name="MountPosition [m]"/>
     <tableColumn id="8" name="MountOrientation [°]"/>
-    <tableColumn id="9" name="InitialOrientation [°]"/>
-    <tableColumn id="10" name="InitialFocal [mm]"/>
-    <tableColumn id="11" name="MinFocal [mm]"/>
-    <tableColumn id="12" name="MaxFocal [mm]"/>
+    <tableColumn id="9" name="InitialFocal [mm]"/>
+    <tableColumn id="10" name="MinFocal [mm]"/>
+    <tableColumn id="11" name="MaxFocal [mm]"/>
   </tableColumns>
 </table>
 </file>
@@ -1260,34 +1248,30 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table2911" displayName="Table2911" ref="A2:G4" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A2:G4"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table2911" displayName="Table2911" ref="A2:F4" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A2:F4"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="GimbalModelID"/>
     <tableColumn id="2" name="GimbalName"/>
     <tableColumn id="3" name="LinkConfigurationID"/>
-    <tableColumn id="4" name="OpticalCenterOffset [mm]"/>
-    <tableColumn id="5" name="Weight [kg]"/>
-    <tableColumn id="6" name="IdlePower [W]"/>
-    <tableColumn id="7" name="ActivePower [W]"/>
+    <tableColumn id="4" name="Weight [kg]"/>
+    <tableColumn id="5" name="IdlePower [W]"/>
+    <tableColumn id="6" name="ActivePower [W]"/>
   </tableColumns>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table291112" displayName="Table291112" ref="A2:J7" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A2:J7"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table291112" displayName="Table291112" ref="A2:G7" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A2:G7"/>
+  <tableColumns count="7">
     <tableColumn id="1" name="GimbalLinkID"/>
     <tableColumn id="2" name="LinkConfigurationID"/>
-    <tableColumn id="3" name="LinkIndex"/>
-    <tableColumn id="4" name="AxisType"/>
-    <tableColumn id="5" name="LinkOffset [mm]"/>
-    <tableColumn id="6" name="LinkLength [mm]"/>
-    <tableColumn id="7" name="JointRange [°]"/>
-    <tableColumn id="8" name="MaxAngularSpeed [°/s]"/>
-    <tableColumn id="9" name="MotorRiseTime [s]"/>
-    <tableColumn id="10" name="MotorDampingFactor"/>
+    <tableColumn id="3" name="AxisType"/>
+    <tableColumn id="4" name="JointRange [°]"/>
+    <tableColumn id="5" name="MaxAngularSpeed [°/s]"/>
+    <tableColumn id="6" name="MotorRiseTime [s]"/>
+    <tableColumn id="7" name="MotorDampingFactor"/>
   </tableColumns>
 </table>
 </file>
@@ -1751,7 +1735,7 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1768,304 +1752,304 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="G2" s="26" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="H2" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="C3" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="D3" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="E3" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="27" t="n">
+        <v>6.287</v>
+      </c>
+      <c r="G3" s="27" t="n">
+        <v>4.712</v>
+      </c>
+      <c r="H3" s="27" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I3" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="J3" s="27" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="C4" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" s="27" t="s">
         <v>220</v>
       </c>
-      <c r="H2" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="B3" s="26" t="s">
+      <c r="E4" s="27" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" s="27" t="n">
+        <v>13.2</v>
+      </c>
+      <c r="G4" s="27" t="n">
+        <v>8.8</v>
+      </c>
+      <c r="H4" s="27" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I4" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="J4" s="27" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="B5" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="C5" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>218</v>
+      </c>
+      <c r="E5" s="27" t="n">
+        <v>30</v>
+      </c>
+      <c r="F5" s="27" t="n">
+        <v>35.9</v>
+      </c>
+      <c r="G5" s="27" t="n">
+        <v>24</v>
+      </c>
+      <c r="H5" s="27" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I5" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="J5" s="27" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="E3" s="26" t="n">
+      <c r="B6" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="E6" s="27" t="n">
+        <v>15</v>
+      </c>
+      <c r="F6" s="27" t="n">
+        <v>17.3</v>
+      </c>
+      <c r="G6" s="27" t="n">
+        <v>13</v>
+      </c>
+      <c r="H6" s="27" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I6" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" s="27" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>218</v>
+      </c>
+      <c r="E7" s="27" t="n">
+        <v>14</v>
+      </c>
+      <c r="F7" s="27" t="n">
+        <v>6.287</v>
+      </c>
+      <c r="G7" s="27" t="n">
+        <v>4.712</v>
+      </c>
+      <c r="H7" s="27" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="I7" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" s="27" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="E8" s="27" t="n">
+        <v>10.27</v>
+      </c>
+      <c r="F8" s="27" t="n">
+        <v>13.2</v>
+      </c>
+      <c r="G8" s="27" t="n">
+        <v>8.8</v>
+      </c>
+      <c r="H8" s="27" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="26" t="n">
-        <v>6.287</v>
-      </c>
-      <c r="G3" s="26" t="n">
-        <v>4.712</v>
-      </c>
-      <c r="H3" s="26" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="I3" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="J3" s="26" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>225</v>
-      </c>
-      <c r="E4" s="26" t="n">
-        <v>10</v>
-      </c>
-      <c r="F4" s="26" t="n">
+      <c r="J8" s="27" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="E9" s="27" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="F9" s="27" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="G9" s="28" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="H9" s="27" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="I9" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="J9" s="27" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="E10" s="27" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="F10" s="27" t="n">
         <v>13.2</v>
       </c>
-      <c r="G4" s="26" t="n">
-        <v>8.8</v>
-      </c>
-      <c r="H4" s="26" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I4" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="J4" s="26" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="26" t="s">
-        <v>226</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>227</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="E5" s="26" t="n">
-        <v>30</v>
-      </c>
-      <c r="F5" s="26" t="n">
-        <v>35.9</v>
-      </c>
-      <c r="G5" s="26" t="n">
-        <v>24</v>
-      </c>
-      <c r="H5" s="26" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="I5" s="26" t="n">
+      <c r="G10" s="27" t="n">
+        <v>7.425</v>
+      </c>
+      <c r="H10" s="27" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="I10" s="27" t="n">
         <v>3</v>
       </c>
-      <c r="J5" s="26" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>225</v>
-      </c>
-      <c r="E6" s="26" t="n">
-        <v>15</v>
-      </c>
-      <c r="F6" s="26" t="n">
-        <v>17.3</v>
-      </c>
-      <c r="G6" s="26" t="n">
-        <v>13</v>
-      </c>
-      <c r="H6" s="26" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I6" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="J6" s="26" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="26" t="s">
-        <v>230</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>231</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="E7" s="26" t="n">
-        <v>14</v>
-      </c>
-      <c r="F7" s="26" t="n">
-        <v>6.287</v>
-      </c>
-      <c r="G7" s="26" t="n">
-        <v>4.712</v>
-      </c>
-      <c r="H7" s="26" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="I7" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="J7" s="26" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="26" t="s">
-        <v>232</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>233</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>234</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>235</v>
-      </c>
-      <c r="E8" s="26" t="n">
-        <v>10.27</v>
-      </c>
-      <c r="F8" s="26" t="n">
-        <v>13.2</v>
-      </c>
-      <c r="G8" s="26" t="n">
-        <v>8.8</v>
-      </c>
-      <c r="H8" s="26" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I8" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" s="26" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>237</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>235</v>
-      </c>
-      <c r="E9" s="26" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="F9" s="26" t="n">
-        <v>6.3</v>
-      </c>
-      <c r="G9" s="27" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="H9" s="26" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="I9" s="26" t="n">
-        <v>3</v>
-      </c>
-      <c r="J9" s="26" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="26" t="s">
-        <v>168</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>239</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>240</v>
-      </c>
-      <c r="E10" s="26" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="F10" s="26" t="n">
-        <v>13.2</v>
-      </c>
-      <c r="G10" s="26" t="n">
-        <v>7.425</v>
-      </c>
-      <c r="H10" s="26" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="I10" s="26" t="n">
-        <v>3</v>
-      </c>
-      <c r="J10" s="26" t="n">
+      <c r="J10" s="27" t="n">
         <v>6</v>
       </c>
     </row>
@@ -2815,21 +2799,21 @@
   </sheetPr>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="2" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="20" width="27.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="27.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="2" width="27.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="14" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="2" width="27.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="24" width="11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16383" min="14" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="2" width="10.49"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
         <v>72</v>
       </c>
@@ -2843,7 +2827,7 @@
       <c r="I1" s="21"/>
       <c r="J1" s="21"/>
       <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
+      <c r="L1" s="2"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
@@ -2871,19 +2855,17 @@
         <v>118</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="L2" s="22" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="3" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="M2" s="24"/>
+    </row>
+    <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
         <v>122</v>
       </c>
@@ -2908,20 +2890,18 @@
       <c r="H3" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="I3" s="23" t="s">
-        <v>89</v>
+      <c r="I3" s="23" t="n">
+        <v>2</v>
       </c>
       <c r="J3" s="23" t="n">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="K3" s="23" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L3" s="23" t="n">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
         <v>129</v>
       </c>
@@ -2946,20 +2926,18 @@
       <c r="H4" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="I4" s="23" t="s">
-        <v>89</v>
+      <c r="I4" s="23" t="n">
+        <v>10</v>
       </c>
       <c r="J4" s="23" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K4" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="L4" s="23" t="n">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
         <v>136</v>
       </c>
@@ -2984,20 +2962,18 @@
       <c r="H5" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="I5" s="23" t="s">
-        <v>89</v>
+      <c r="I5" s="23" t="n">
+        <v>10</v>
       </c>
       <c r="J5" s="23" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K5" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="L5" s="23" t="n">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
         <v>139</v>
       </c>
@@ -3022,20 +2998,18 @@
       <c r="H6" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="I6" s="23" t="s">
-        <v>89</v>
+      <c r="I6" s="23" t="n">
+        <v>10</v>
       </c>
       <c r="J6" s="23" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K6" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="L6" s="23" t="n">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
         <v>143</v>
       </c>
@@ -3060,20 +3034,18 @@
       <c r="H7" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="I7" s="23" t="s">
-        <v>89</v>
+      <c r="I7" s="23" t="n">
+        <v>2</v>
       </c>
       <c r="J7" s="23" t="n">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="K7" s="23" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L7" s="23" t="n">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="s">
         <v>145</v>
       </c>
@@ -3098,20 +3070,18 @@
       <c r="H8" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="I8" s="23" t="s">
-        <v>89</v>
+      <c r="I8" s="23" t="n">
+        <v>10</v>
       </c>
       <c r="J8" s="23" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K8" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="L8" s="23" t="n">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="23" t="s">
         <v>147</v>
       </c>
@@ -3136,20 +3106,18 @@
       <c r="H9" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="I9" s="23" t="s">
-        <v>89</v>
+      <c r="I9" s="23" t="n">
+        <v>2</v>
       </c>
       <c r="J9" s="23" t="n">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="K9" s="23" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L9" s="23" t="n">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="23" t="s">
         <v>149</v>
       </c>
@@ -3174,20 +3142,18 @@
       <c r="H10" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="I10" s="23" t="s">
-        <v>89</v>
+      <c r="I10" s="23" t="n">
+        <v>2</v>
       </c>
       <c r="J10" s="23" t="n">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="K10" s="23" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L10" s="23" t="n">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="23" t="s">
         <v>151</v>
       </c>
@@ -3212,20 +3178,18 @@
       <c r="H11" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="I11" s="23" t="s">
-        <v>89</v>
+      <c r="I11" s="23" t="n">
+        <v>2</v>
       </c>
       <c r="J11" s="23" t="n">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="K11" s="23" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L11" s="23" t="n">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
         <v>154</v>
       </c>
@@ -3250,20 +3214,18 @@
       <c r="H12" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="I12" s="23" t="s">
-        <v>89</v>
+      <c r="I12" s="23" t="n">
+        <v>10</v>
       </c>
       <c r="J12" s="23" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K12" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="L12" s="23" t="n">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="23" t="s">
         <v>157</v>
       </c>
@@ -3288,20 +3250,18 @@
       <c r="H13" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="I13" s="23" t="s">
-        <v>89</v>
+      <c r="I13" s="23" t="n">
+        <v>10</v>
       </c>
       <c r="J13" s="23" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K13" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="L13" s="23" t="n">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="23" t="s">
         <v>159</v>
       </c>
@@ -3326,20 +3286,18 @@
       <c r="H14" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="I14" s="23" t="s">
-        <v>89</v>
+      <c r="I14" s="23" t="n">
+        <v>10</v>
       </c>
       <c r="J14" s="23" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K14" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="L14" s="23" t="n">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" s="2" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="s">
         <v>162</v>
       </c>
@@ -3364,18 +3322,16 @@
       <c r="H15" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="I15" s="23" t="s">
-        <v>89</v>
+      <c r="I15" s="23" t="n">
+        <v>10</v>
       </c>
       <c r="J15" s="23" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K15" s="23" t="n">
-        <v>8</v>
-      </c>
-      <c r="L15" s="23" t="n">
         <v>40</v>
       </c>
+      <c r="L15" s="2"/>
     </row>
     <row r="16" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="s">
@@ -3402,19 +3358,17 @@
       <c r="H16" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="I16" s="23" t="s">
-        <v>128</v>
+      <c r="I16" s="23" t="n">
+        <v>2</v>
       </c>
       <c r="J16" s="23" t="n">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="K16" s="23" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="L16" s="23" t="n">
         <v>12</v>
       </c>
-      <c r="M16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="24"/>
     </row>
     <row r="17" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3435,7 +3389,7 @@
     <row r="33" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3470,112 +3424,112 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="26" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="D3" s="26" t="n">
+      <c r="D3" s="27" t="n">
         <v>10</v>
       </c>
-      <c r="E3" s="26" t="n">
+      <c r="E3" s="27" t="n">
         <v>15</v>
       </c>
-      <c r="F3" s="26" t="n">
+      <c r="F3" s="27" t="n">
         <v>4.5</v>
       </c>
-      <c r="G3" s="26" t="n">
+      <c r="G3" s="27" t="n">
         <v>1.5</v>
       </c>
-      <c r="H3" s="26" t="n">
+      <c r="H3" s="27" t="n">
         <v>250</v>
       </c>
-      <c r="I3" s="26" t="n">
+      <c r="I3" s="27" t="n">
         <v>200</v>
       </c>
-      <c r="J3" s="26" t="n">
+      <c r="J3" s="27" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="27" t="s">
         <v>183</v>
       </c>
-      <c r="D4" s="26" t="n">
+      <c r="D4" s="27" t="n">
         <v>8</v>
       </c>
-      <c r="E4" s="26" t="n">
+      <c r="E4" s="27" t="n">
         <v>12</v>
       </c>
-      <c r="F4" s="26" t="n">
+      <c r="F4" s="27" t="n">
         <v>6.5</v>
       </c>
-      <c r="G4" s="26" t="n">
+      <c r="G4" s="27" t="n">
         <v>2.5</v>
       </c>
-      <c r="H4" s="26" t="n">
+      <c r="H4" s="27" t="n">
         <v>400</v>
       </c>
-      <c r="I4" s="26" t="n">
+      <c r="I4" s="27" t="n">
         <v>350</v>
       </c>
-      <c r="J4" s="26" t="n">
+      <c r="J4" s="27" t="n">
         <v>25</v>
       </c>
     </row>
@@ -3620,92 +3574,85 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="2" width="29.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="2" width="29.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="24" width="11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16383" min="8" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="2" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="26" t="s">
         <v>188</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="24"/>
+    </row>
+    <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="B3" s="26" t="s">
+      <c r="C3" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="D3" s="27" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E3" s="27" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3" s="27" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="C4" s="27" t="s">
         <v>192</v>
       </c>
-      <c r="E3" s="26" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="F3" s="26" t="n">
-        <v>5</v>
-      </c>
-      <c r="G3" s="26" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>192</v>
-      </c>
-      <c r="E4" s="26" t="n">
+      <c r="D4" s="27" t="n">
         <v>0.6</v>
       </c>
-      <c r="F4" s="26" t="n">
+      <c r="E4" s="27" t="n">
         <v>10</v>
       </c>
-      <c r="G4" s="26" t="n">
+      <c r="F4" s="27" t="n">
         <v>20</v>
       </c>
     </row>
@@ -3724,7 +3671,7 @@
     <row r="17" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3746,219 +3693,168 @@
   </sheetPr>
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="2" width="28"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="11" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="2" width="28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="24" width="10.49"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="9" style="24" width="11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16381" min="11" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="2" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="D2" s="26" t="s">
         <v>195</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="C2" s="25" t="s">
+      <c r="E2" s="26" t="s">
         <v>196</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="F2" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="G2" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+    </row>
+    <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="27" t="s">
         <v>199</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="B3" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="D3" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="E3" s="27" t="n">
+        <v>180</v>
+      </c>
+      <c r="F3" s="27" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G3" s="27" t="n">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="B4" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="27" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="s">
+      <c r="D4" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>191</v>
-      </c>
-      <c r="C3" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="26" t="s">
+      <c r="E4" s="27" t="n">
+        <v>180</v>
+      </c>
+      <c r="F4" s="27" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="G4" s="27" t="n">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="27" t="s">
         <v>205</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="B5" s="27" t="s">
         <v>192</v>
       </c>
-      <c r="F3" s="26" t="n">
-        <v>50</v>
-      </c>
-      <c r="G3" s="26" t="s">
+      <c r="C5" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="H3" s="26" t="n">
+      <c r="D5" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="E5" s="27" t="n">
         <v>270</v>
       </c>
-      <c r="I3" s="26" t="n">
+      <c r="F5" s="27" t="n">
         <v>0.06</v>
       </c>
-      <c r="J3" s="26" t="n">
+      <c r="G5" s="27" t="n">
         <v>0.95</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>191</v>
-      </c>
-      <c r="C4" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" s="26" t="s">
+    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="27" t="s">
         <v>208</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="B6" s="27" t="s">
         <v>192</v>
       </c>
-      <c r="F4" s="26" t="n">
-        <v>50</v>
-      </c>
-      <c r="G4" s="26" t="s">
+      <c r="C6" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="E6" s="27" t="n">
+        <v>180</v>
+      </c>
+      <c r="F6" s="27" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G6" s="27" t="n">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="H4" s="26" t="n">
+      <c r="B7" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="E7" s="27" t="n">
         <v>180</v>
       </c>
-      <c r="I4" s="26" t="n">
+      <c r="F7" s="27" t="n">
         <v>0.05</v>
       </c>
-      <c r="J4" s="26" t="n">
-        <v>0.97</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="C5" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>205</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>192</v>
-      </c>
-      <c r="F5" s="26" t="n">
-        <v>50</v>
-      </c>
-      <c r="G5" s="26" t="s">
-        <v>206</v>
-      </c>
-      <c r="H5" s="26" t="n">
-        <v>270</v>
-      </c>
-      <c r="I5" s="26" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="J5" s="26" t="n">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="26" t="s">
-        <v>211</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="C6" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>212</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>192</v>
-      </c>
-      <c r="F6" s="26" t="n">
-        <v>50</v>
-      </c>
-      <c r="G6" s="26" t="s">
-        <v>213</v>
-      </c>
-      <c r="H6" s="26" t="n">
-        <v>180</v>
-      </c>
-      <c r="I6" s="26" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="J6" s="26" t="n">
-        <v>0.97</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="26" t="s">
-        <v>214</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="C7" s="26" t="n">
-        <v>3</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="E7" s="26" t="s">
-        <v>192</v>
-      </c>
-      <c r="F7" s="26" t="n">
-        <v>50</v>
-      </c>
-      <c r="G7" s="26" t="s">
-        <v>209</v>
-      </c>
-      <c r="H7" s="26" t="n">
-        <v>180</v>
-      </c>
-      <c r="I7" s="26" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="J7" s="26" t="n">
+      <c r="G7" s="27" t="n">
         <v>0.99</v>
       </c>
     </row>
@@ -3978,7 +3874,7 @@
     <row r="21" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Add settings for Unreal lumen
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Missions" sheetId="1" state="visible" r:id="rId3"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="242">
   <si>
     <t xml:space="preserve">GENERAL CONFIGURATION</t>
   </si>
@@ -148,6 +148,9 @@
     <t xml:space="preserve">DrawWorldMarkers</t>
   </si>
   <si>
+    <t xml:space="preserve">EnableLumen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Slow Simple</t>
   </si>
   <si>
@@ -536,6 +539,9 @@
   </si>
   <si>
     <t xml:space="preserve">CAM07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=0.0, Y=0.0, Z=-0.05)</t>
   </si>
   <si>
     <t xml:space="preserve">HARDWARE CATALOGS</t>
@@ -1759,7 +1765,7 @@
   </sheetPr>
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -1779,7 +1785,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -1795,54 +1801,54 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="L2" s="25" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E3" s="26" t="n">
         <v>1</v>
@@ -1854,10 +1860,10 @@
         <v>4.712</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="J3" s="26" t="n">
         <v>0.2</v>
@@ -1871,16 +1877,16 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="E4" s="26" t="n">
         <v>10</v>
@@ -1892,10 +1898,10 @@
         <v>8.8</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="I4" s="26" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="J4" s="26" t="n">
         <v>0.5</v>
@@ -1909,16 +1915,16 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="26" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E5" s="26" t="n">
         <v>30</v>
@@ -1930,10 +1936,10 @@
         <v>24</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="I5" s="26" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="J5" s="26" t="n">
         <v>0.6</v>
@@ -1947,16 +1953,16 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="26" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="E6" s="26" t="n">
         <v>15</v>
@@ -1968,10 +1974,10 @@
         <v>13</v>
       </c>
       <c r="H6" s="26" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="I6" s="26" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="J6" s="26" t="n">
         <v>0.5</v>
@@ -1985,16 +1991,16 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="26" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E7" s="26" t="n">
         <v>14</v>
@@ -2006,10 +2012,10 @@
         <v>4.712</v>
       </c>
       <c r="H7" s="26" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="I7" s="26" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="J7" s="26" t="n">
         <v>0.4</v>
@@ -2023,16 +2029,16 @@
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="26" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E8" s="26" t="n">
         <v>10.27</v>
@@ -2044,10 +2050,10 @@
         <v>8.8</v>
       </c>
       <c r="H8" s="26" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="I8" s="26" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="J8" s="26" t="n">
         <v>0.5</v>
@@ -2061,16 +2067,16 @@
     </row>
     <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="26" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B9" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="D9" s="26" t="s">
         <v>236</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>237</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>234</v>
       </c>
       <c r="E9" s="26" t="n">
         <v>5.5</v>
@@ -2082,10 +2088,10 @@
         <v>4.7</v>
       </c>
       <c r="H9" s="26" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="J9" s="26" t="n">
         <v>0.8</v>
@@ -2099,16 +2105,16 @@
     </row>
     <row r="10" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="26" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="E10" s="26" t="n">
         <v>4.5</v>
@@ -2120,10 +2126,10 @@
         <v>7.425</v>
       </c>
       <c r="H10" s="26" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="I10" s="26" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="J10" s="26" t="n">
         <v>0.8</v>
@@ -2171,17 +2177,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="2" width="26.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="2" width="11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2194,6 +2200,7 @@
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
@@ -2217,13 +2224,16 @@
       <c r="G2" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="H2" s="6" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>20</v>
@@ -2243,13 +2253,17 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="H3" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>20</v>
@@ -2269,16 +2283,20 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="H4" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D5" s="9" t="n">
         <v>1</v>
@@ -2292,6 +2310,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="17" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="10" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2311,7 +2333,7 @@
     <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="15"/>
       <c r="D9" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E9" s="14"/>
     </row>
@@ -2377,22 +2399,22 @@
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2400,22 +2422,22 @@
         <v>16</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2465,71 +2487,71 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E3" s="19" t="n">
         <v>16</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E4" s="19" t="n">
         <v>16</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2580,7 +2602,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -2595,64 +2617,64 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I3" s="23" t="n">
         <v>4</v>
@@ -2666,28 +2688,28 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B4" s="23" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I4" s="23" t="n">
         <v>4</v>
@@ -2701,28 +2723,28 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I5" s="23" t="n">
         <v>4</v>
@@ -2736,28 +2758,28 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I6" s="23" t="n">
         <v>4</v>
@@ -2771,28 +2793,28 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I7" s="23" t="n">
         <v>3</v>
@@ -2806,28 +2828,28 @@
     </row>
     <row r="8" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I8" s="23" t="n">
         <v>3</v>
@@ -2881,8 +2903,8 @@
   </sheetPr>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2897,7 +2919,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -2913,64 +2935,64 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M2" s="20"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I3" s="23" t="n">
         <v>2</v>
@@ -2985,28 +3007,28 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I4" s="23" t="n">
         <v>10</v>
@@ -3021,28 +3043,28 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I5" s="23" t="n">
         <v>10</v>
@@ -3057,28 +3079,28 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I6" s="23" t="n">
         <v>10</v>
@@ -3093,28 +3115,28 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I7" s="23" t="n">
         <v>2</v>
@@ -3129,28 +3151,28 @@
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I8" s="23" t="n">
         <v>10</v>
@@ -3165,28 +3187,28 @@
     </row>
     <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="23" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H9" s="23" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I9" s="23" t="n">
         <v>2</v>
@@ -3201,28 +3223,28 @@
     </row>
     <row r="10" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="23" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I10" s="23" t="n">
         <v>2</v>
@@ -3237,28 +3259,28 @@
     </row>
     <row r="11" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="23" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H11" s="23" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I11" s="23" t="n">
         <v>2</v>
@@ -3273,28 +3295,28 @@
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H12" s="23" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I12" s="23" t="n">
         <v>10</v>
@@ -3309,28 +3331,28 @@
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="23" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H13" s="23" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I13" s="23" t="n">
         <v>10</v>
@@ -3345,28 +3367,28 @@
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="23" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H14" s="23" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I14" s="23" t="n">
         <v>10</v>
@@ -3381,28 +3403,28 @@
     </row>
     <row r="15" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H15" s="23" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I15" s="23" t="n">
         <v>10</v>
@@ -3417,28 +3439,28 @@
     </row>
     <row r="16" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>127</v>
+        <v>170</v>
       </c>
       <c r="H16" s="23" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I16" s="23" t="n">
         <v>2</v>
@@ -3507,7 +3529,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -3521,45 +3543,45 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D3" s="26" t="n">
         <v>10</v>
@@ -3585,13 +3607,13 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D4" s="26" t="n">
         <v>8</v>
@@ -3669,7 +3691,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -3679,34 +3701,34 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G2" s="20"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D3" s="26" t="n">
         <v>0.4</v>
@@ -3720,13 +3742,13 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D4" s="26" t="n">
         <v>0.6</v>
@@ -3790,7 +3812,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -3801,25 +3823,25 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
@@ -3827,16 +3849,16 @@
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E3" s="26" t="n">
         <v>180</v>
@@ -3850,16 +3872,16 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E4" s="26" t="n">
         <v>180</v>
@@ -3873,16 +3895,16 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="26" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E5" s="26" t="n">
         <v>270</v>
@@ -3896,16 +3918,16 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="26" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E6" s="26" t="n">
         <v>180</v>
@@ -3919,16 +3941,16 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="26" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E7" s="26" t="n">
         <v>180</v>

</xml_diff>

<commit_message>
Add sensor params (Barometer, IMU, GPS, Magnetometer)
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Missions" sheetId="1" state="visible" r:id="rId3"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="250">
   <si>
     <t xml:space="preserve">GENERAL CONFIGURATION</t>
   </si>
@@ -202,7 +202,7 @@
     <t xml:space="preserve">(17:00:00)</t>
   </si>
   <si>
-    <t xml:space="preserve">(Vx=0.0, Vy=0.0, Vz=0.0)</t>
+    <t xml:space="preserve">(Vx=5.0, Vy=3.5, Vz=0.8)</t>
   </si>
   <si>
     <t xml:space="preserve">GroupID</t>
@@ -280,6 +280,18 @@
     <t xml:space="preserve">MaxAltitude [m]</t>
   </si>
   <si>
+    <t xml:space="preserve">Barometer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnetometer</t>
+  </si>
+  <si>
     <t xml:space="preserve">BatteryCapacity [mAh]</t>
   </si>
   <si>
@@ -302,6 +314,18 @@
   </si>
   <si>
     <t xml:space="preserve">(Pitch=0.0, Yaw=0.0, Roll=0.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(PressureSigma=0.0001825, NoiseSigma=3.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(GyroNoise=0.4, AccelNoise=0.2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(EphIni=30, EpvIni=40, EphFin=1, EpvFin=2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(NoiseSigma=0.03, ScaleFactor=1.02, NoiseBias=0.05)</t>
   </si>
   <si>
     <t xml:space="preserve">AGENT01</t>
@@ -1189,9 +1213,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A2:K7" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A2:K7"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A2:O7" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A2:O7"/>
+  <tableColumns count="15">
     <tableColumn id="1" name="AgentID"/>
     <tableColumn id="2" name="AgentTeamID"/>
     <tableColumn id="3" name="AgentName"/>
@@ -1202,7 +1226,11 @@
     <tableColumn id="8" name="InitialOrientation [°]"/>
     <tableColumn id="9" name="SafetyRadius [m]"/>
     <tableColumn id="10" name="MaxAltitude [m]"/>
-    <tableColumn id="11" name="BatteryCapacity [mAh]"/>
+    <tableColumn id="11" name="Barometer"/>
+    <tableColumn id="12" name="IMU"/>
+    <tableColumn id="13" name="GPS"/>
+    <tableColumn id="14" name="Magnetometer"/>
+    <tableColumn id="15" name="BatteryCapacity [mAh]"/>
   </tableColumns>
 </table>
 </file>
@@ -1785,7 +1813,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -1801,54 +1829,54 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="L2" s="25" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="E3" s="26" t="n">
         <v>1</v>
@@ -1860,10 +1888,10 @@
         <v>4.712</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="J3" s="26" t="n">
         <v>0.2</v>
@@ -1877,16 +1905,16 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="E4" s="26" t="n">
         <v>10</v>
@@ -1898,10 +1926,10 @@
         <v>8.8</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="I4" s="26" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="J4" s="26" t="n">
         <v>0.5</v>
@@ -1915,16 +1943,16 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="26" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="E5" s="26" t="n">
         <v>30</v>
@@ -1936,10 +1964,10 @@
         <v>24</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="I5" s="26" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="J5" s="26" t="n">
         <v>0.6</v>
@@ -1953,16 +1981,16 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="26" t="s">
+        <v>237</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="C6" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>230</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>221</v>
-      </c>
       <c r="D6" s="26" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="E6" s="26" t="n">
         <v>15</v>
@@ -1974,10 +2002,10 @@
         <v>13</v>
       </c>
       <c r="H6" s="26" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="I6" s="26" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="J6" s="26" t="n">
         <v>0.5</v>
@@ -1991,16 +2019,16 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="26" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="E7" s="26" t="n">
         <v>14</v>
@@ -2012,10 +2040,10 @@
         <v>4.712</v>
       </c>
       <c r="H7" s="26" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="I7" s="26" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="J7" s="26" t="n">
         <v>0.4</v>
@@ -2029,16 +2057,16 @@
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="26" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="E8" s="26" t="n">
         <v>10.27</v>
@@ -2050,10 +2078,10 @@
         <v>8.8</v>
       </c>
       <c r="H8" s="26" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="I8" s="26" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="J8" s="26" t="n">
         <v>0.5</v>
@@ -2067,16 +2095,16 @@
     </row>
     <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="26" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="E9" s="26" t="n">
         <v>5.5</v>
@@ -2088,10 +2116,10 @@
         <v>4.7</v>
       </c>
       <c r="H9" s="26" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="J9" s="26" t="n">
         <v>0.8</v>
@@ -2105,16 +2133,16 @@
     </row>
     <row r="10" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="26" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="E10" s="26" t="n">
         <v>4.5</v>
@@ -2126,10 +2154,10 @@
         <v>7.425</v>
       </c>
       <c r="H10" s="26" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="I10" s="26" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="J10" s="26" t="n">
         <v>0.8</v>
@@ -2371,8 +2399,8 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2583,10 +2611,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N14" activeCellId="0" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2596,8 +2624,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="29.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="32.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="9" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="14" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="44.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="40.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="52.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="56.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="18" style="2" width="11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2614,6 +2647,10 @@
       <c r="I1" s="21"/>
       <c r="J1" s="21"/>
       <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
@@ -2649,32 +2686,44 @@
       <c r="K2" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="M2" s="12"/>
+      <c r="L2" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="N2" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="O2" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I3" s="23" t="n">
         <v>4</v>
@@ -2682,34 +2731,46 @@
       <c r="J3" s="23" t="n">
         <v>250</v>
       </c>
-      <c r="K3" s="23" t="n">
+      <c r="K3" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="L3" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="M3" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="N3" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="O3" s="23" t="n">
         <v>10000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="B4" s="23" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>88</v>
-      </c>
       <c r="G4" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" s="23" t="s">
         <v>94</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>90</v>
       </c>
       <c r="I4" s="23" t="n">
         <v>4</v>
@@ -2717,34 +2778,46 @@
       <c r="J4" s="23" t="n">
         <v>250</v>
       </c>
-      <c r="K4" s="23" t="n">
+      <c r="K4" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="L4" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="M4" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="O4" s="23" t="n">
         <v>10000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I5" s="23" t="n">
         <v>4</v>
@@ -2752,34 +2825,46 @@
       <c r="J5" s="23" t="n">
         <v>250</v>
       </c>
-      <c r="K5" s="23" t="n">
+      <c r="K5" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="L5" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="M5" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="N5" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="O5" s="23" t="n">
         <v>10000</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I6" s="23" t="n">
         <v>4</v>
@@ -2787,34 +2872,46 @@
       <c r="J6" s="23" t="n">
         <v>250</v>
       </c>
-      <c r="K6" s="23" t="n">
+      <c r="K6" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="L6" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="M6" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="N6" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="O6" s="23" t="n">
         <v>10000</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I7" s="23" t="n">
         <v>3</v>
@@ -2822,34 +2919,46 @@
       <c r="J7" s="23" t="n">
         <v>300</v>
       </c>
-      <c r="K7" s="23" t="n">
+      <c r="K7" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="L7" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="M7" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="N7" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="O7" s="23" t="n">
         <v>12000</v>
       </c>
     </row>
     <row r="8" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I8" s="23" t="n">
         <v>3</v>
@@ -2857,10 +2966,22 @@
       <c r="J8" s="23" t="n">
         <v>300</v>
       </c>
-      <c r="K8" s="23" t="n">
+      <c r="K8" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="L8" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="M8" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="N8" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="O8" s="23" t="n">
         <v>12000</v>
       </c>
-      <c r="L8" s="2"/>
+      <c r="P8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2881,7 +3002,7 @@
     <row r="25" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:O1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2903,7 +3024,7 @@
   </sheetPr>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -2935,64 +3056,64 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>76</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="M2" s="20"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="I3" s="23" t="n">
         <v>2</v>
@@ -3007,28 +3128,28 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="I4" s="23" t="n">
         <v>10</v>
@@ -3043,28 +3164,28 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="H5" s="23" t="s">
         <v>137</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>129</v>
       </c>
       <c r="I5" s="23" t="n">
         <v>10</v>
@@ -3079,28 +3200,28 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="B6" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" s="23" t="s">
+      <c r="E6" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>133</v>
-      </c>
       <c r="F6" s="23" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="I6" s="23" t="n">
         <v>10</v>
@@ -3115,28 +3236,28 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="I7" s="23" t="n">
         <v>2</v>
@@ -3151,28 +3272,28 @@
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="I8" s="23" t="n">
         <v>10</v>
@@ -3187,28 +3308,28 @@
     </row>
     <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="23" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H9" s="23" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="I9" s="23" t="n">
         <v>2</v>
@@ -3223,28 +3344,28 @@
     </row>
     <row r="10" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="23" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="I10" s="23" t="n">
         <v>2</v>
@@ -3259,28 +3380,28 @@
     </row>
     <row r="11" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="23" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H11" s="23" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="I11" s="23" t="n">
         <v>2</v>
@@ -3295,28 +3416,28 @@
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="H12" s="23" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="I12" s="23" t="n">
         <v>10</v>
@@ -3331,28 +3452,28 @@
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="23" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="H13" s="23" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="I13" s="23" t="n">
         <v>10</v>
@@ -3367,28 +3488,28 @@
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="23" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="H14" s="23" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="I14" s="23" t="n">
         <v>10</v>
@@ -3403,28 +3524,28 @@
     </row>
     <row r="15" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="H15" s="23" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="I15" s="23" t="n">
         <v>10</v>
@@ -3439,28 +3560,28 @@
     </row>
     <row r="16" s="12" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="H16" s="23" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="I16" s="23" t="n">
         <v>2</v>
@@ -3529,7 +3650,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -3546,42 +3667,42 @@
         <v>78</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="D3" s="26" t="n">
         <v>10</v>
@@ -3607,13 +3728,13 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="D4" s="26" t="n">
         <v>8</v>
@@ -3691,7 +3812,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -3701,34 +3822,34 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="G2" s="20"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="D3" s="26" t="n">
         <v>0.4</v>
@@ -3742,13 +3863,13 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="D4" s="26" t="n">
         <v>0.6</v>
@@ -3812,7 +3933,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -3823,25 +3944,25 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>187</v>
-      </c>
       <c r="C2" s="25" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
@@ -3849,16 +3970,16 @@
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="E3" s="26" t="n">
         <v>180</v>
@@ -3872,16 +3993,16 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="E4" s="26" t="n">
         <v>180</v>
@@ -3895,16 +4016,16 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="26" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="E5" s="26" t="n">
         <v>270</v>
@@ -3918,16 +4039,16 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="C6" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>202</v>
-      </c>
       <c r="D6" s="26" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="E6" s="26" t="n">
         <v>180</v>
@@ -3941,16 +4062,16 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="26" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="E7" s="26" t="n">
         <v>180</v>

</xml_diff>

<commit_message>
Add trajectories and update tracking parameters
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Mission" sheetId="1" state="visible" r:id="rId3"/>
@@ -14,9 +14,10 @@
     <sheet name="Agent" sheetId="4" state="visible" r:id="rId6"/>
     <sheet name="Tracking" sheetId="5" state="visible" r:id="rId7"/>
     <sheet name="Head" sheetId="6" state="visible" r:id="rId8"/>
-    <sheet name="Drone" sheetId="7" state="visible" r:id="rId9"/>
-    <sheet name="Gimbal" sheetId="8" state="visible" r:id="rId10"/>
-    <sheet name="Camera" sheetId="9" state="visible" r:id="rId11"/>
+    <sheet name="Window" sheetId="7" state="visible" r:id="rId9"/>
+    <sheet name="Drone" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="Gimbal" sheetId="9" state="visible" r:id="rId11"/>
+    <sheet name="Camera" sheetId="10" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="193">
   <si>
     <t xml:space="preserve">GENERAL CONFIGURATION</t>
   </si>
@@ -165,7 +166,7 @@
     <t xml:space="preserve">High</t>
   </si>
   <si>
-    <t xml:space="preserve">VeryLowSpeedHighDispersion16</t>
+    <t xml:space="preserve">LowSpeedLowDispersion8</t>
   </si>
   <si>
     <t xml:space="preserve">TARGET01</t>
@@ -186,16 +187,16 @@
     <t xml:space="preserve">Slow, Low Dispersion, 12 Humans</t>
   </si>
   <si>
-    <t xml:space="preserve">VeryLowSpeedLowDispersion8</t>
-  </si>
-  <si>
     <t xml:space="preserve">AGENT CONFIGURATION</t>
   </si>
   <si>
     <t xml:space="preserve">TrackingID</t>
   </si>
   <si>
-    <t xml:space="preserve">HeadPayloadID</t>
+    <t xml:space="preserve">HeadSetID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WindowSetID</t>
   </si>
   <si>
     <t xml:space="preserve">DroneID</t>
@@ -225,7 +226,10 @@
     <t xml:space="preserve">TRACKING00</t>
   </si>
   <si>
-    <t xml:space="preserve">PAYLOAD00</t>
+    <t xml:space="preserve">HEADSET00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
   </si>
   <si>
     <t xml:space="preserve">DRONE00</t>
@@ -243,25 +247,25 @@
     <t xml:space="preserve">Multi-Camera-Tracking Agent</t>
   </si>
   <si>
+    <t xml:space="preserve">HEADSET01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DRONE01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGENT02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-Window-Tracking Agent</t>
+  </si>
+  <si>
     <t xml:space="preserve">TRACKING01</t>
   </si>
   <si>
-    <t xml:space="preserve">PAYLOAD01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DRONE01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGENT02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multi-Window-Tracking Agent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRACKING02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAYLOAD02</t>
+    <t xml:space="preserve">HEADSET02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WINDOWSET00</t>
   </si>
   <si>
     <t xml:space="preserve">Mode</t>
@@ -276,280 +280,298 @@
     <t xml:space="preserve">RefTargetSize</t>
   </si>
   <si>
-    <t xml:space="preserve">NumWindows</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SceneResolution [pix]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TrackingResolution [pix]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default Tracking</t>
+    <t xml:space="preserve">Default Camera Tracking</t>
   </si>
   <si>
     <t xml:space="preserve">MultiCamera</t>
   </si>
   <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multi-Camera-Tracking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multi-Window-Tracking</t>
+    <t xml:space="preserve">Default Window Tracking</t>
   </si>
   <si>
     <t xml:space="preserve">MultiWindow</t>
   </si>
   <si>
+    <t xml:space="preserve">GimbalID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CameraID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MinFocal [mm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxFocal [mm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RefFocal [mm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default Head</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIM00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAM00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tracking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=0.0, Y=0.0, Z=-0.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Roll=0.0, Pitch=90.0, Yaw=0.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-Camera Tracking Cam 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAM01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=0.3, Y=0.0, Z=-0.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-Camera Tracking Cam 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=0.0, Y=0.3, Z=-0.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Roll=0.0, Pitch=90.0, Yaw=90.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-Camera Tracking Cam 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=-0.3, Y=0.0, Z=-0.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Roll=0.0, Pitch=90.0, Yaw=180.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-Camera Tracking Cam 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(X=0.0, Y=-0.3, Z=-0.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Roll=0.0, Pitch=90.0, Yaw=270.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-Camera Central Cam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAM02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-Window Central Cam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAM03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MinLambda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxLambda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RefLambda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resolution [pix]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WINDOW00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-Window Tracking Window 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(240x135)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WINDOW01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-Window Tracking Window 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WINDOW02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-Window Tracking Window 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WINDOW03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-Window Tracking Window 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HARDWARE CATALOGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CruiseSpeed [m/s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxSpeed [m/s]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnableBarometer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barometer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnableIMU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnableGPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnableMagnetometer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnetometer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BaseWeight [kg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxPayloadWeight [kg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HoverPower [W]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CruisePower [W]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LoadFactor [W/kg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default Drone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quadcopter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(PressureSigma=0.0001825, NoiseSigma=3.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(GyroNoise=0.4, AccelNoise=0.2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(EphIni=30, EpvIni=40, EphFin=1, EpvFin=2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(NoiseSigma=0.03, ScaleFactor=1.02, NoiseBias=0.05)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DJI S900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hexacopter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnableRoll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnablePitch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pitch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnableYaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weight [kg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IdlePower [W]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ActivePower [W]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default Gimbal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Min=-20.0, Max=20.0, Speed=180)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Min=-40.0, Max=130.0, Speed=180)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Min=-320.0, Max=320.0, Speed=270)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SensorSize [mm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnableLensDistortion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LensDistortion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnableSensorNoise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SensorNoise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default Camera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGB</t>
+  </si>
+  <si>
     <t xml:space="preserve">(1280x720)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(480x270)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GimbalID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CameraID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Role</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MinFocal [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxFocal [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RefFocal [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default Head</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIM00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAM00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tracking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=0.0, Y=0.0, Z=-0.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Roll=0.0, Pitch=90.0, Yaw=0.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multi-Camera Tracking Cam 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAM01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=0.3, Y=0.0, Z=-0.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multi-Camera Tracking Cam 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=0.0, Y=0.3, Z=-0.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Roll=0.0, Pitch=90.0, Yaw=90.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multi-Camera Tracking Cam 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=-0.3, Y=0.0, Z=-0.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Roll=0.0, Pitch=90.0, Yaw=180.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multi-Camera Tracking Cam 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(X=0.0, Y=-0.3, Z=-0.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Roll=0.0, Pitch=90.0, Yaw=270.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multi-Camera Central Cam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAM02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multi-Window Central Cam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAM03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HARDWARE CATALOGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CruiseSpeed [m/s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxSpeed [m/s]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnableBarometer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Barometer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnableIMU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnableGPS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnableMagnetometer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magnetometer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BaseWeight [kg]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxPayloadWeight [kg]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HoverPower [W]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CruisePower [W]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LoadFactor [W/kg]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default Drone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quadcopter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(PressureSigma=0.0001825, NoiseSigma=3.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(GyroNoise=0.4, AccelNoise=0.2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(EphIni=30, EpvIni=40, EphFin=1, EpvFin=2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(NoiseSigma=0.03, ScaleFactor=1.02, NoiseBias=0.05)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DJI S900</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hexacopter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnableRoll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnablePitch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pitch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnableYaw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yaw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weight [kg]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IdlePower [W]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ActivePower [W]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default Gimbal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Min=-20.0, Max=20.0, Speed=180)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Min=-40.0, Max=130.0, Speed=180)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Min=-320.0, Max=320.0, Speed=270)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resolution [pix]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SensorSize [mm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnableLensDistortion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LensDistortion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnableSensorNoise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SensorNoise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default Camera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RGB</t>
   </si>
   <si>
     <t xml:space="preserve">(13.2x8.8)</t>
@@ -752,7 +774,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -830,10 +852,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -987,20 +1005,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A2:K3" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A2:K3"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A2:L3" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A2:L3"/>
+  <tableColumns count="12">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="3" name="AgentTeamID"/>
     <tableColumn id="4" name="TrackingID"/>
-    <tableColumn id="5" name="HeadPayloadID"/>
-    <tableColumn id="6" name="DroneID"/>
-    <tableColumn id="7" name="Position [m]"/>
-    <tableColumn id="8" name="Orientation [°]"/>
-    <tableColumn id="9" name="MaxAltitude [m]"/>
-    <tableColumn id="10" name="SafetyRadius [m]"/>
-    <tableColumn id="11" name="BatteryCapacity [mAh]"/>
+    <tableColumn id="5" name="HeadSetID"/>
+    <tableColumn id="6" name="WindowSetID"/>
+    <tableColumn id="7" name="DroneID"/>
+    <tableColumn id="8" name="Position [m]"/>
+    <tableColumn id="9" name="Orientation [°]"/>
+    <tableColumn id="10" name="MaxAltitude [m]"/>
+    <tableColumn id="11" name="SafetyRadius [m]"/>
+    <tableColumn id="12" name="BatteryCapacity [mAh]"/>
+  </tableColumns>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table72" displayName="Table72" ref="A2:G3" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A2:G3"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="ID2"/>
+    <tableColumn id="2" name="ID"/>
+    <tableColumn id="3" name="Name"/>
+    <tableColumn id="4" name="EnvironmentID"/>
+    <tableColumn id="5" name="TargetGroupID"/>
+    <tableColumn id="6" name="AgentTeamID"/>
+    <tableColumn id="7" name="AltitudeConstraint [m]"/>
   </tableColumns>
 </table>
 </file>
@@ -1011,7 +1045,7 @@
   <tableColumns count="10">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Name"/>
-    <tableColumn id="3" name="HeadPayloadID"/>
+    <tableColumn id="3" name="HeadSetID"/>
     <tableColumn id="4" name="GimbalID"/>
     <tableColumn id="5" name="CameraID"/>
     <tableColumn id="6" name="Role"/>
@@ -1024,7 +1058,21 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table29" displayName="Table29" ref="A2:L5" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table210_2" displayName="Table210_2" ref="A2:F6" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A2:F6"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="2" name="Name"/>
+    <tableColumn id="3" name="WindowSetID"/>
+    <tableColumn id="4" name="MinLambda"/>
+    <tableColumn id="5" name="MaxLambda"/>
+    <tableColumn id="6" name="RefLambda"/>
+  </tableColumns>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table29" displayName="Table29" ref="A2:L5" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A2:L5"/>
   <tableColumns count="12">
     <tableColumn id="1" name="ID"/>
@@ -1043,8 +1091,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table2911" displayName="Table2911" ref="A2:K3" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table2911" displayName="Table2911" ref="A2:K3" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A2:K3"/>
   <tableColumns count="11">
     <tableColumn id="1" name="ID"/>
@@ -1062,8 +1110,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table2913" displayName="Table2913" ref="A2:R4" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table2913" displayName="Table2913" ref="A2:R4" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A2:R4"/>
   <tableColumns count="18">
     <tableColumn id="1" name="ID"/>
@@ -1088,25 +1136,22 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table2_2" displayName="Table2_2" ref="A2:I3" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A2:I3"/>
-  <tableColumns count="9">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table2_2" displayName="Table2_2" ref="A2:F3" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A2:F3"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="3" name="Mode"/>
     <tableColumn id="4" name="MinTargetSize"/>
     <tableColumn id="5" name="MaxTargetSize"/>
     <tableColumn id="6" name="RefTargetSize"/>
-    <tableColumn id="7" name="NumWindows"/>
-    <tableColumn id="8" name="SceneResolution [pix]"/>
-    <tableColumn id="9" name="TrackingResolution [pix]"/>
   </tableColumns>
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table5" displayName="Table5" ref="A2:G2" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table5" displayName="Table5" ref="A2:G2" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A2:G2"/>
   <tableColumns count="7">
     <tableColumn id="1" name="ID"/>
@@ -1120,29 +1165,14 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table6" displayName="Table6" ref="A2:D3" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table6" displayName="Table6" ref="A2:D3" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A2:D3"/>
   <tableColumns count="4">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="3" name="Geopoint"/>
     <tableColumn id="4" name="WindVel [m/s]"/>
-  </tableColumns>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table72" displayName="Table72" ref="A2:G3" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A2:G3"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="ID2"/>
-    <tableColumn id="2" name="ID"/>
-    <tableColumn id="3" name="Name"/>
-    <tableColumn id="4" name="EnvironmentID"/>
-    <tableColumn id="5" name="TargetGroupID"/>
-    <tableColumn id="6" name="AgentTeamID"/>
-    <tableColumn id="7" name="AltitudeConstraint [m]"/>
   </tableColumns>
 </table>
 </file>
@@ -1606,6 +1636,280 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="true"/>
+  </sheetPr>
+  <dimension ref="A1:XFD20"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="39.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="32.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="68.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="30.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="68.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="30.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16382" min="13" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="3" width="10.49"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+    </row>
+    <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="XFC2" s="3"/>
+      <c r="XFD2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="F3" s="22" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="H3" s="22" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J3" s="22" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="22" t="n">
+        <v>2</v>
+      </c>
+      <c r="L3" s="22" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="F4" s="22" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="H4" s="22" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J4" s="22" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K4" s="22" t="n">
+        <v>2</v>
+      </c>
+      <c r="L4" s="22" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="F5" s="22" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="H5" s="22" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J5" s="22" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K5" s="22" t="n">
+        <v>2</v>
+      </c>
+      <c r="L5" s="22" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="F6" s="22" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="H6" s="22" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="J6" s="22" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K6" s="22" t="n">
+        <v>3</v>
+      </c>
+      <c r="L6" s="22" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:L1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="8" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <tableParts>
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1706,8 +2010,8 @@
   </sheetPr>
   <dimension ref="A1:BM9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1778,7 +2082,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
         <v>46</v>
       </c>
@@ -1857,8 +2161,9 @@
       <c r="BJ4" s="12"/>
       <c r="BK4" s="12"/>
       <c r="BL4" s="12"/>
-    </row>
-    <row r="5" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="BM4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
         <v>50</v>
       </c>
@@ -1878,7 +2183,7 @@
         <v>44</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
@@ -1937,6 +2242,7 @@
       <c r="BJ5" s="12"/>
       <c r="BK5" s="12"/>
       <c r="BL5" s="12"/>
+      <c r="BM5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1964,10 +2270,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:XFD22"/>
+  <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1975,22 +2281,21 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="38.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="12" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="29.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="36.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="29.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="13" style="12" width="11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16380" min="18" style="2" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16383" min="16381" style="2" width="10.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="3" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="12" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="29.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="36.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="29.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="14" style="12" width="11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16381" min="19" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="2" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -2002,6 +2307,7 @@
       <c r="I1" s="17"/>
       <c r="J1" s="17"/>
       <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
@@ -2014,35 +2320,37 @@
         <v>5</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="G2" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="H2" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="I2" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="J2" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="K2" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="L2" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="M2" s="12"/>
       <c r="N2" s="12"/>
       <c r="O2" s="12"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
-      <c r="XFD2" s="3"/>
+      <c r="R2" s="12"/>
     </row>
     <row r="3" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
@@ -2069,64 +2377,64 @@
       <c r="H3" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="I3" s="19" t="n">
+      <c r="I3" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" s="19" t="n">
         <v>300</v>
       </c>
-      <c r="J3" s="19" t="n">
+      <c r="K3" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="K3" s="19" t="n">
+      <c r="L3" s="19" t="n">
         <v>12000</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="12"/>
+      <c r="M3" s="2"/>
       <c r="N3" s="12"/>
       <c r="O3" s="12"/>
       <c r="P3" s="12"/>
       <c r="Q3" s="12"/>
       <c r="R3" s="12"/>
       <c r="S3" s="12"/>
-      <c r="XFA3" s="2"/>
-      <c r="XFB3" s="2"/>
-      <c r="XFC3" s="2"/>
+      <c r="T3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E4" s="19" t="s">
         <v>72</v>
       </c>
       <c r="F4" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="19" t="s">
         <v>73</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>67</v>
       </c>
       <c r="H4" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="I4" s="19" t="n">
+      <c r="I4" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" s="19" t="n">
         <v>300</v>
       </c>
-      <c r="J4" s="19" t="n">
+      <c r="K4" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="K4" s="19" t="n">
+      <c r="L4" s="19" t="n">
         <v>12000</v>
       </c>
-      <c r="XFA4" s="3"/>
-      <c r="XFB4" s="3"/>
-      <c r="XFC4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
@@ -2145,21 +2453,24 @@
         <v>77</v>
       </c>
       <c r="F5" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="19" t="s">
         <v>73</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>67</v>
       </c>
       <c r="H5" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="I5" s="19" t="n">
+      <c r="I5" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" s="19" t="n">
         <v>300</v>
       </c>
-      <c r="J5" s="19" t="n">
+      <c r="K5" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="K5" s="19" t="n">
+      <c r="L5" s="19" t="n">
         <v>12000</v>
       </c>
     </row>
@@ -2182,7 +2493,7 @@
     <row r="22" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2202,10 +2513,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:XFD22"/>
+  <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2215,27 +2526,22 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="12" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="29.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="32.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="2" width="28.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="11" style="12" width="11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16378" min="16" style="2" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16381" min="16379" style="2" width="10.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="3" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="8" style="12" width="11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16375" min="13" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16378" min="16376" style="2" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16379" style="3" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
       <c r="E1" s="17"/>
       <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
@@ -2245,31 +2551,25 @@
         <v>2</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="H2" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>84</v>
-      </c>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
+      <c r="XEY2" s="3"/>
+      <c r="XEZ2" s="3"/>
+      <c r="XFA2" s="3"/>
       <c r="XFB2" s="3"/>
       <c r="XFC2" s="3"/>
       <c r="XFD2" s="3"/>
@@ -2279,10 +2579,10 @@
         <v>64</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D3" s="19" t="n">
         <v>0.2</v>
@@ -2293,33 +2593,24 @@
       <c r="F3" s="19" t="n">
         <v>0.8</v>
       </c>
-      <c r="G3" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="J3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="12"/>
       <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="XEY3" s="2"/>
-      <c r="XEZ3" s="2"/>
-      <c r="XFA3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="XEV3" s="2"/>
+      <c r="XEW3" s="2"/>
+      <c r="XEX3" s="2"/>
+    </row>
+    <row r="4" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>86</v>
@@ -2331,50 +2622,21 @@
         <v>0.9</v>
       </c>
       <c r="F4" s="19" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="I4" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="XEY4" s="3"/>
-      <c r="XEZ4" s="3"/>
-      <c r="XFA4" s="3"/>
-    </row>
-    <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" s="19" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E5" s="19" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="F5" s="19" t="n">
         <v>0.7</v>
       </c>
-      <c r="G5" s="19" t="n">
-        <v>4</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="I5" s="20" t="s">
-        <v>92</v>
-      </c>
-    </row>
+      <c r="G4" s="2"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="XEV4" s="2"/>
+      <c r="XEW4" s="2"/>
+      <c r="XEX4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2390,11 +2652,11 @@
     <row r="18" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2416,8 +2678,8 @@
   </sheetPr>
   <dimension ref="A1:XFD26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2435,7 +2697,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -2457,16 +2719,16 @@
         <v>2</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G2" s="18" t="s">
         <v>57</v>
@@ -2475,13 +2737,13 @@
         <v>58</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="M2" s="12"/>
       <c r="N2" s="3"/>
@@ -2489,28 +2751,28 @@
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>65</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="I3" s="19" t="n">
         <v>8</v>
@@ -2525,28 +2787,28 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>72</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F4" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="G4" s="19" t="s">
-        <v>109</v>
-      </c>
       <c r="H4" s="19" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="I4" s="19" t="n">
         <v>8</v>
@@ -2561,28 +2823,28 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>72</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="I5" s="19" t="n">
         <v>8</v>
@@ -2597,28 +2859,28 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>72</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="I6" s="19" t="n">
         <v>8</v>
@@ -2633,28 +2895,28 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>72</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="I7" s="19" t="n">
         <v>8</v>
@@ -2669,28 +2931,28 @@
     </row>
     <row r="8" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="19" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>72</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="I8" s="19" t="n">
         <v>1</v>
@@ -2706,28 +2968,28 @@
     </row>
     <row r="9" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>77</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="I9" s="19" t="n">
         <v>1</v>
@@ -2780,6 +3042,196 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
+  <dimension ref="A1:XFD23"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="38.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="2" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="12" width="27.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16375" min="8" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16376" style="3" width="10.49"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+    </row>
+    <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="XEV2" s="3"/>
+      <c r="XEW2" s="3"/>
+      <c r="XEX2" s="3"/>
+      <c r="XEY2" s="3"/>
+      <c r="XEZ2" s="3"/>
+      <c r="XFA2" s="3"/>
+      <c r="XFB2" s="3"/>
+      <c r="XFC2" s="3"/>
+      <c r="XFD2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="19" t="n">
+        <v>0.167</v>
+      </c>
+      <c r="E3" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="19" t="n">
+        <v>0.583</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="19" t="n">
+        <v>0.167</v>
+      </c>
+      <c r="E4" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="19" t="n">
+        <v>0.583</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="19" t="n">
+        <v>0.167</v>
+      </c>
+      <c r="E5" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="19" t="n">
+        <v>0.583</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="19" t="n">
+        <v>0.167</v>
+      </c>
+      <c r="E6" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="19" t="n">
+        <v>0.583</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="8" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <tableParts>
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="true"/>
+  </sheetPr>
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -2804,200 +3256,200 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
+      <c r="A1" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="K2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="N2" s="22" t="s">
+      <c r="G2" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="H2" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="P2" s="22" t="s">
+      <c r="I2" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="Q2" s="22" t="s">
+      <c r="J2" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="R2" s="22" t="s">
+      <c r="K2" s="21" t="s">
         <v>144</v>
       </c>
+      <c r="L2" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q2" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="R2" s="21" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="D3" s="23" t="n">
+      <c r="A3" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="22" t="n">
         <v>10</v>
       </c>
-      <c r="E3" s="23" t="n">
+      <c r="E3" s="22" t="n">
         <v>15</v>
       </c>
-      <c r="F3" s="23" t="b">
+      <c r="F3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G3" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="H3" s="23" t="b">
+      <c r="G3" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="H3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I3" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="J3" s="23" t="b">
+      <c r="I3" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="J3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K3" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="L3" s="23" t="b">
+      <c r="K3" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="L3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="M3" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="N3" s="23" t="n">
+      <c r="M3" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="N3" s="22" t="n">
         <v>4.5</v>
       </c>
-      <c r="O3" s="23" t="n">
+      <c r="O3" s="22" t="n">
         <v>1.5</v>
       </c>
-      <c r="P3" s="23" t="n">
+      <c r="P3" s="22" t="n">
         <v>250</v>
       </c>
-      <c r="Q3" s="23" t="n">
+      <c r="Q3" s="22" t="n">
         <v>200</v>
       </c>
-      <c r="R3" s="23" t="n">
+      <c r="R3" s="22" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="D4" s="23" t="n">
+      <c r="B4" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="E4" s="23" t="n">
+      <c r="E4" s="22" t="n">
         <v>12</v>
       </c>
-      <c r="F4" s="23" t="b">
+      <c r="F4" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G4" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="H4" s="23" t="b">
+      <c r="G4" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="H4" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I4" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="J4" s="23" t="b">
+      <c r="I4" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="J4" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K4" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="L4" s="23" t="b">
+      <c r="K4" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="L4" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="M4" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="N4" s="23" t="n">
+      <c r="M4" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="N4" s="22" t="n">
         <v>6.5</v>
       </c>
-      <c r="O4" s="23" t="n">
+      <c r="O4" s="22" t="n">
         <v>2.5</v>
       </c>
-      <c r="P4" s="23" t="n">
+      <c r="P4" s="22" t="n">
         <v>400</v>
       </c>
-      <c r="Q4" s="23" t="n">
+      <c r="Q4" s="22" t="n">
         <v>350</v>
       </c>
-      <c r="R4" s="23" t="n">
+      <c r="R4" s="22" t="n">
         <v>25</v>
       </c>
     </row>
@@ -3034,7 +3486,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
@@ -3059,92 +3511,92 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
+      <c r="A1" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="J2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>161</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>168</v>
       </c>
       <c r="L2" s="12"/>
       <c r="XFD2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C3" s="23" t="b">
+      <c r="A3" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="E3" s="23" t="b">
+      <c r="D3" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="E3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F3" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="G3" s="23" t="b">
+      <c r="F3" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="G3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H3" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="I3" s="23" t="n">
+      <c r="H3" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="I3" s="22" t="n">
         <v>0.4</v>
       </c>
-      <c r="J3" s="23" t="n">
+      <c r="J3" s="22" t="n">
         <v>5</v>
       </c>
-      <c r="K3" s="23" t="n">
+      <c r="K3" s="22" t="n">
         <v>15</v>
       </c>
     </row>
@@ -3176,278 +3628,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="true"/>
-  </sheetPr>
-  <dimension ref="A1:XFD20"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="39.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="32.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="68.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="30.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="68.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="30.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16382" min="13" style="2" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="3" width="10.49"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-    </row>
-    <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="L2" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="XFC2" s="3"/>
-      <c r="XFD2" s="3"/>
-    </row>
-    <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>172</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="F3" s="23" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="H3" s="23" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I3" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="J3" s="23" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K3" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="L3" s="23" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="F4" s="23" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G4" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="H4" s="23" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I4" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="J4" s="23" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K4" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="L4" s="23" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="F5" s="23" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="H5" s="23" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I5" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="J5" s="23" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="K5" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="L5" s="23" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="F6" s="23" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="H6" s="23" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I6" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="J6" s="23" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="K6" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="L6" s="23" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="8" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <tableParts>
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Make central window have the same a fixed resolution factor
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="194">
   <si>
     <t xml:space="preserve">GENERAL CONFIGURATION</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t xml:space="preserve">Slow, Low Dispersion, 12 Humans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LowSpeedHighDispersion8</t>
   </si>
   <si>
     <t xml:space="preserve">AGENT CONFIGURATION</t>
@@ -1665,7 +1668,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -1690,64 +1693,64 @@
         <v>37</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="L2" s="21" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="XFC2" s="3"/>
       <c r="XFD2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="J3" s="22" t="n">
         <v>0.5</v>
@@ -1761,33 +1764,33 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F4" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H4" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="J4" s="22" t="n">
         <v>0.5</v>
@@ -1801,33 +1804,33 @@
     </row>
     <row r="5" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F5" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H5" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="J5" s="22" t="n">
         <v>0.2</v>
@@ -1841,33 +1844,33 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="22" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F6" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H6" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="J6" s="22" t="n">
         <v>0.8</v>
@@ -2011,7 +2014,7 @@
   <dimension ref="A1:BM9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2183,7 +2186,7 @@
         <v>44</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
@@ -2295,7 +2298,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -2320,31 +2323,31 @@
         <v>5</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N2" s="12"/>
       <c r="O2" s="12"/>
@@ -2354,31 +2357,31 @@
     </row>
     <row r="3" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J3" s="19" t="n">
         <v>300</v>
@@ -2400,31 +2403,31 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J4" s="19" t="n">
         <v>300</v>
@@ -2438,31 +2441,31 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J5" s="19" t="n">
         <v>300</v>
@@ -2535,7 +2538,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -2551,16 +2554,16 @@
         <v>2</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
@@ -2576,13 +2579,13 @@
     </row>
     <row r="3" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D3" s="19" t="n">
         <v>0.2</v>
@@ -2607,13 +2610,13 @@
     </row>
     <row r="4" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D4" s="19" t="n">
         <v>0.2</v>
@@ -2697,7 +2700,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -2719,31 +2722,31 @@
         <v>2</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M2" s="12"/>
       <c r="N2" s="3"/>
@@ -2751,28 +2754,28 @@
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I3" s="19" t="n">
         <v>8</v>
@@ -2787,28 +2790,28 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="19" t="s">
         <v>100</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>99</v>
       </c>
       <c r="I4" s="19" t="n">
         <v>8</v>
@@ -2823,28 +2826,28 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I5" s="19" t="n">
         <v>8</v>
@@ -2859,28 +2862,28 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I6" s="19" t="n">
         <v>8</v>
@@ -2895,28 +2898,28 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I7" s="19" t="n">
         <v>8</v>
@@ -2931,28 +2934,28 @@
     </row>
     <row r="8" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="19" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I8" s="19" t="n">
         <v>1</v>
@@ -2968,28 +2971,28 @@
     </row>
     <row r="9" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="B9" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>119</v>
-      </c>
       <c r="G9" s="19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I9" s="19" t="n">
         <v>1</v>
@@ -3060,7 +3063,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -3077,19 +3080,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="XEV2" s="3"/>
       <c r="XEW2" s="3"/>
@@ -3103,13 +3106,13 @@
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D3" s="19" t="n">
         <v>0.167</v>
@@ -3121,18 +3124,18 @@
         <v>0.583</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D4" s="19" t="n">
         <v>0.167</v>
@@ -3144,18 +3147,18 @@
         <v>0.583</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D5" s="19" t="n">
         <v>0.167</v>
@@ -3167,18 +3170,18 @@
         <v>0.583</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D6" s="19" t="n">
         <v>0.167</v>
@@ -3190,7 +3193,7 @@
         <v>0.583</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3257,7 +3260,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -3288,60 +3291,60 @@
         <v>37</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="L2" s="21" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="M2" s="21" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="O2" s="21" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="P2" s="21" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="Q2" s="21" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="R2" s="21" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D3" s="22" t="n">
         <v>10</v>
@@ -3354,28 +3357,28 @@
         <v>1</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="K3" s="22" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M3" s="22" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N3" s="22" t="n">
         <v>4.5</v>
@@ -3395,13 +3398,13 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D4" s="22" t="n">
         <v>8</v>
@@ -3414,28 +3417,28 @@
         <v>1</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H4" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J4" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="K4" s="22" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L4" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M4" s="22" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N4" s="22" t="n">
         <v>6.5</v>
@@ -3512,7 +3515,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -3533,62 +3536,62 @@
         <v>2</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="L2" s="12"/>
       <c r="XFD2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I3" s="22" t="n">
         <v>0.4</v>

</xml_diff>

<commit_message>
Add central and tracking cost parameters for agent positioning
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -187,7 +187,7 @@
     <t xml:space="preserve">Slow, Low Dispersion, 12 Humans</t>
   </si>
   <si>
-    <t xml:space="preserve">LowSpeedHighDispersion8</t>
+    <t xml:space="preserve">MedSpeedHighDispersion8</t>
   </si>
   <si>
     <t xml:space="preserve">AGENT CONFIGURATION</t>
@@ -385,25 +385,7 @@
     <t xml:space="preserve">HEAD05</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Multi-Camera Central </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Head</t>
-    </r>
+    <t xml:space="preserve">Multi-Camera Central Head</t>
   </si>
   <si>
     <t xml:space="preserve">CAM02</t>
@@ -415,25 +397,7 @@
     <t xml:space="preserve">HEAD06</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Multi-Window Central </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Head</t>
-    </r>
+    <t xml:space="preserve">Multi-Window Central Head</t>
   </si>
   <si>
     <t xml:space="preserve">CAM03</t>
@@ -664,7 +628,7 @@
     <numFmt numFmtId="165" formatCode="h:mm:ss"/>
     <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -732,12 +696,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -825,7 +783,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -903,10 +861,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1721,218 +1675,218 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="L2" s="21" t="s">
         <v>172</v>
       </c>
       <c r="XFC2" s="3"/>
       <c r="XFD2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="F3" s="23" t="b">
+      <c r="F3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H3" s="23" t="b">
+      <c r="H3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="J3" s="23" t="n">
+      <c r="J3" s="22" t="n">
         <v>0.5</v>
       </c>
-      <c r="K3" s="23" t="n">
+      <c r="K3" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="L3" s="23" t="n">
+      <c r="L3" s="22" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="F4" s="23" t="b">
+      <c r="F4" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H4" s="23" t="b">
+      <c r="H4" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="J4" s="23" t="n">
+      <c r="J4" s="22" t="n">
         <v>0.5</v>
       </c>
-      <c r="K4" s="23" t="n">
+      <c r="K4" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="L4" s="23" t="n">
+      <c r="L4" s="22" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="5" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="F5" s="23" t="b">
+      <c r="F5" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H5" s="23" t="b">
+      <c r="H5" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="J5" s="23" t="n">
+      <c r="J5" s="22" t="n">
         <v>0.2</v>
       </c>
-      <c r="K5" s="23" t="n">
+      <c r="K5" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="L5" s="23" t="n">
+      <c r="L5" s="22" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="22" t="s">
         <v>193</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="22" t="s">
         <v>194</v>
       </c>
-      <c r="F6" s="23" t="b">
+      <c r="F6" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H6" s="23" t="b">
+      <c r="H6" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="J6" s="23" t="n">
+      <c r="J6" s="22" t="n">
         <v>0.8</v>
       </c>
-      <c r="K6" s="23" t="n">
+      <c r="K6" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="L6" s="23" t="n">
+      <c r="L6" s="22" t="n">
         <v>6</v>
       </c>
     </row>
@@ -2068,7 +2022,7 @@
   <dimension ref="A1:BM9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3102,7 +3056,7 @@
   <dimension ref="A1:XFD21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3114,8 +3068,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="27.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="12" width="27.34"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16376" min="9" style="2" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16383" min="16377" style="3" width="10.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16377" style="3" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3162,7 +3115,7 @@
       <c r="XFA2" s="3"/>
       <c r="XFB2" s="3"/>
       <c r="XFC2" s="3"/>
-      <c r="XFD2" s="0"/>
+      <c r="XFD2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
@@ -3183,19 +3136,12 @@
       <c r="F3" s="19" t="n">
         <v>0.167</v>
       </c>
-      <c r="G3" s="20" t="n">
+      <c r="G3" s="19" t="n">
         <v>0.167</v>
       </c>
-      <c r="H3" s="20" t="n">
+      <c r="H3" s="19" t="n">
         <v>0.167</v>
       </c>
-      <c r="XEW3" s="0"/>
-      <c r="XEX3" s="0"/>
-      <c r="XEY3" s="0"/>
-      <c r="XEZ3" s="0"/>
-      <c r="XFA3" s="0"/>
-      <c r="XFB3" s="0"/>
-      <c r="XFC3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
@@ -3361,200 +3307,200 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="L2" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="M2" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="N2" s="22" t="s">
+      <c r="N2" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="O2" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="P2" s="22" t="s">
+      <c r="P2" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="Q2" s="22" t="s">
+      <c r="Q2" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="R2" s="22" t="s">
+      <c r="R2" s="21" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="D3" s="23" t="n">
+      <c r="D3" s="22" t="n">
         <v>10</v>
       </c>
-      <c r="E3" s="23" t="n">
+      <c r="E3" s="22" t="n">
         <v>15</v>
       </c>
-      <c r="F3" s="23" t="b">
+      <c r="F3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="H3" s="23" t="b">
+      <c r="H3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="J3" s="23" t="b">
+      <c r="J3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="L3" s="23" t="b">
+      <c r="L3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="M3" s="23" t="s">
+      <c r="M3" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="N3" s="23" t="n">
+      <c r="N3" s="22" t="n">
         <v>4.5</v>
       </c>
-      <c r="O3" s="23" t="n">
+      <c r="O3" s="22" t="n">
         <v>1.5</v>
       </c>
-      <c r="P3" s="23" t="n">
+      <c r="P3" s="22" t="n">
         <v>250</v>
       </c>
-      <c r="Q3" s="23" t="n">
+      <c r="Q3" s="22" t="n">
         <v>200</v>
       </c>
-      <c r="R3" s="23" t="n">
+      <c r="R3" s="22" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="D4" s="23" t="n">
+      <c r="D4" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="E4" s="23" t="n">
+      <c r="E4" s="22" t="n">
         <v>12</v>
       </c>
-      <c r="F4" s="23" t="b">
+      <c r="F4" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="H4" s="23" t="b">
+      <c r="H4" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="J4" s="23" t="b">
+      <c r="J4" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K4" s="23" t="s">
+      <c r="K4" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="L4" s="23" t="b">
+      <c r="L4" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="M4" s="23" t="s">
+      <c r="M4" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="N4" s="23" t="n">
+      <c r="N4" s="22" t="n">
         <v>6.5</v>
       </c>
-      <c r="O4" s="23" t="n">
+      <c r="O4" s="22" t="n">
         <v>2.5</v>
       </c>
-      <c r="P4" s="23" t="n">
+      <c r="P4" s="22" t="n">
         <v>400</v>
       </c>
-      <c r="Q4" s="23" t="n">
+      <c r="Q4" s="22" t="n">
         <v>350</v>
       </c>
-      <c r="R4" s="23" t="n">
+      <c r="R4" s="22" t="n">
         <v>25</v>
       </c>
     </row>
@@ -3616,92 +3562,92 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="21" t="s">
         <v>172</v>
       </c>
       <c r="L2" s="12"/>
       <c r="XFD2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="C3" s="23" t="b">
+      <c r="C3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="E3" s="23" t="b">
+      <c r="E3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="G3" s="23" t="b">
+      <c r="G3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="I3" s="23" t="n">
+      <c r="I3" s="22" t="n">
         <v>0.4</v>
       </c>
-      <c r="J3" s="23" t="n">
+      <c r="J3" s="22" t="n">
         <v>5</v>
       </c>
-      <c r="K3" s="23" t="n">
+      <c r="K3" s="22" t="n">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add camera distortion parameters
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Mission" sheetId="1" state="visible" r:id="rId3"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="195">
   <si>
     <t xml:space="preserve">GENERAL CONFIGURATION</t>
   </si>
@@ -565,10 +565,7 @@
     <t xml:space="preserve">SensorSize [mm]</t>
   </si>
   <si>
-    <t xml:space="preserve">EnableLensDistortion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LensDistortion</t>
+    <t xml:space="preserve">Distortion (K1, K2, K3, P1, P2)</t>
   </si>
   <si>
     <t xml:space="preserve">EnableSensorNoise</t>
@@ -586,7 +583,7 @@
     <t xml:space="preserve">(13.2x8.8)</t>
   </si>
   <si>
-    <t xml:space="preserve">(Strength=0.02, Radius=1.8, Falloff=0.15)</t>
+    <t xml:space="preserve">(-0.03, 0.002, 0.0, 0.0005, -0.0004)</t>
   </si>
   <si>
     <t xml:space="preserve">(RandContrib=0.008, RandSize=500, RandSpeed=50000)</t>
@@ -1083,21 +1080,20 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table29" displayName="Table29" ref="A2:L5" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A2:L5"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table29" displayName="Table29" ref="A2:K5" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A2:K5"/>
+  <tableColumns count="11">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="3" name="Type"/>
     <tableColumn id="4" name="Resolution [pix]"/>
     <tableColumn id="5" name="SensorSize [mm]"/>
-    <tableColumn id="6" name="EnableLensDistortion"/>
-    <tableColumn id="7" name="LensDistortion"/>
-    <tableColumn id="8" name="EnableSensorNoise"/>
-    <tableColumn id="9" name="SensorNoise"/>
-    <tableColumn id="10" name="Weight [kg]"/>
-    <tableColumn id="11" name="IdlePower [W]"/>
-    <tableColumn id="12" name="ActivePower [W]"/>
+    <tableColumn id="6" name="Distortion (K1, K2, K3, P1, P2)"/>
+    <tableColumn id="7" name="EnableSensorNoise"/>
+    <tableColumn id="8" name="SensorNoise"/>
+    <tableColumn id="9" name="Weight [kg]"/>
+    <tableColumn id="10" name="IdlePower [W]"/>
+    <tableColumn id="11" name="ActivePower [W]"/>
   </tableColumns>
 </table>
 </file>
@@ -1654,8 +1650,8 @@
   </sheetPr>
   <dimension ref="A1:XFD20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1663,14 +1659,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="39.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="32.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="68.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="30.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="68.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="30.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="26.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16382" min="13" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="54.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="30.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="68.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="30.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="26.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16381" min="12" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16382" min="16382" style="0" width="10.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="3" width="10.49"/>
   </cols>
   <sheetData>
@@ -1688,7 +1684,6 @@
       <c r="I1" s="20"/>
       <c r="J1" s="20"/>
       <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
@@ -1716,17 +1711,15 @@
         <v>180</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="L2" s="21" t="s">
         <v>172</v>
       </c>
+      <c r="XFB2" s="0"/>
       <c r="XFC2" s="3"/>
       <c r="XFD2" s="3"/>
     </row>
@@ -1735,38 +1728,34 @@
         <v>97</v>
       </c>
       <c r="B3" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>182</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>183</v>
       </c>
       <c r="D3" s="22" t="s">
         <v>130</v>
       </c>
       <c r="E3" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="F3" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="F3" s="22" t="b">
+      <c r="G3" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="H3" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H3" s="22" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I3" s="22" t="s">
-        <v>186</v>
+      <c r="I3" s="22" t="n">
+        <v>0.5</v>
       </c>
       <c r="J3" s="22" t="n">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="K3" s="22" t="n">
-        <v>2</v>
-      </c>
-      <c r="L3" s="22" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1775,38 +1764,34 @@
         <v>103</v>
       </c>
       <c r="B4" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="D4" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="E4" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="D4" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="E4" s="22" t="s">
+      <c r="F4" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="F4" s="22" t="b">
+      <c r="G4" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="H4" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H4" s="22" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I4" s="22" t="s">
-        <v>186</v>
+      <c r="I4" s="22" t="n">
+        <v>0.5</v>
       </c>
       <c r="J4" s="22" t="n">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="K4" s="22" t="n">
-        <v>2</v>
-      </c>
-      <c r="L4" s="22" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1815,78 +1800,71 @@
         <v>119</v>
       </c>
       <c r="B5" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="D5" s="22" t="s">
+      <c r="E5" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="E5" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="F5" s="22" t="b">
+      <c r="F5" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="G5" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="H5" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="H5" s="22" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I5" s="22" t="s">
-        <v>186</v>
+      <c r="I5" s="22" t="n">
+        <v>0.2</v>
       </c>
       <c r="J5" s="22" t="n">
-        <v>0.2</v>
+        <v>2</v>
       </c>
       <c r="K5" s="22" t="n">
-        <v>2</v>
-      </c>
-      <c r="L5" s="22" t="n">
         <v>5</v>
       </c>
+      <c r="XFB5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="22" t="s">
         <v>123</v>
       </c>
       <c r="B6" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="D6" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="C6" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="D6" s="22" t="s">
+      <c r="E6" s="22" t="s">
         <v>193</v>
       </c>
-      <c r="E6" s="22" t="s">
-        <v>194</v>
-      </c>
-      <c r="F6" s="22" t="b">
+      <c r="F6" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="G6" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G6" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="H6" s="22" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I6" s="22" t="s">
-        <v>195</v>
+      <c r="H6" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="I6" s="22" t="n">
+        <v>0.8</v>
       </c>
       <c r="J6" s="22" t="n">
-        <v>0.8</v>
+        <v>3</v>
       </c>
       <c r="K6" s="22" t="n">
-        <v>3</v>
-      </c>
-      <c r="L6" s="22" t="n">
         <v>6</v>
       </c>
     </row>
@@ -1906,7 +1884,7 @@
     <row r="20" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2283,7 +2261,7 @@
   </sheetPr>
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix multi-camera tracking agent coordination
</commit_message>
<xml_diff>
--- a/config/Configuration.xlsx
+++ b/config/Configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Mission" sheetId="1" state="visible" r:id="rId3"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="195">
   <si>
     <t xml:space="preserve">GENERAL CONFIGURATION</t>
   </si>
@@ -94,6 +94,9 @@
     <t xml:space="preserve">(14:30:00)</t>
   </si>
   <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
     <t xml:space="preserve">MISSION01</t>
   </si>
   <si>
@@ -115,9 +118,6 @@
     <t xml:space="preserve">(16:30:00)</t>
   </si>
   <si>
-    <t xml:space="preserve">X</t>
-  </si>
-  <si>
     <t xml:space="preserve">MISSION02</t>
   </si>
   <si>
@@ -343,6 +343,21 @@
     <t xml:space="preserve">HEAD01</t>
   </si>
   <si>
+    <t xml:space="preserve">Multi-Camera Central Head</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAM02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Roll=0.0, Pitch=90.0, Yaw=90.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEAD02</t>
+  </si>
+  <si>
     <t xml:space="preserve">Multi-Camera Tracking Head 1</t>
   </si>
   <si>
@@ -352,7 +367,7 @@
     <t xml:space="preserve">(X=0.3, Y=0.0, Z=-0.15)</t>
   </si>
   <si>
-    <t xml:space="preserve">HEAD02</t>
+    <t xml:space="preserve">HEAD03</t>
   </si>
   <si>
     <t xml:space="preserve">Multi-Camera Tracking Head 2</t>
@@ -361,10 +376,7 @@
     <t xml:space="preserve">(X=0.0, Y=0.3, Z=-0.15)</t>
   </si>
   <si>
-    <t xml:space="preserve">(Roll=0.0, Pitch=90.0, Yaw=90.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEAD03</t>
+    <t xml:space="preserve">HEAD04</t>
   </si>
   <si>
     <t xml:space="preserve">Multi-Camera Tracking Head 3</t>
@@ -376,7 +388,7 @@
     <t xml:space="preserve">(Roll=0.0, Pitch=90.0, Yaw=180.0)</t>
   </si>
   <si>
-    <t xml:space="preserve">HEAD04</t>
+    <t xml:space="preserve">HEAD05</t>
   </si>
   <si>
     <t xml:space="preserve">Multi-Camera Tracking Head 4</t>
@@ -388,18 +400,6 @@
     <t xml:space="preserve">(Roll=0.0, Pitch=90.0, Yaw=270.0)</t>
   </si>
   <si>
-    <t xml:space="preserve">HEAD05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multi-Camera Central Head</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAM02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central</t>
-  </si>
-  <si>
     <t xml:space="preserve">HEAD06</t>
   </si>
   <si>
@@ -586,13 +586,13 @@
     <t xml:space="preserve">RGB</t>
   </si>
   <si>
-    <t xml:space="preserve">(13.2x8.8)</t>
+    <t xml:space="preserve">(13.2x7.425)</t>
   </si>
   <si>
     <t xml:space="preserve">(-0.03, 0.002, 0.0, 0.0005, -0.0004)</t>
   </si>
   <si>
-    <t xml:space="preserve">(RandContrib=0.008, RandSize=500, RandSpeed=50000)</t>
+    <t xml:space="preserve">(RandContrib=0.001, RandSize=100, RandSpeed=50000)</t>
   </si>
   <si>
     <t xml:space="preserve">Mavic 2 Pro (Mod. Zoom)</t>
@@ -607,19 +607,13 @@
     <t xml:space="preserve">(2560x1440)</t>
   </si>
   <si>
-    <t xml:space="preserve">(6.287x4.712)</t>
+    <t xml:space="preserve">(6.287x3.536)</t>
   </si>
   <si>
     <t xml:space="preserve">Ultra-High-Resolution Camera</t>
   </si>
   <si>
     <t xml:space="preserve">(7680x4320)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(13.2x7.425)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(RandContrib=0.001, RandSize=100, RandSpeed=50000)</t>
   </si>
 </sst>
 </file>
@@ -900,7 +894,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFDAE3F3"/>
+          <fgColor rgb="FF000000"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -908,7 +902,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
+          <fgColor rgb="FFDAE3F3"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -1370,8 +1364,8 @@
   </sheetPr>
   <dimension ref="A1:XFD19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1472,21 +1466,23 @@
       </c>
     </row>
     <row r="4" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8"/>
+      <c r="A4" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="B4" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>16</v>
@@ -1495,13 +1491,13 @@
         <v>17</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>19</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
@@ -1550,9 +1546,7 @@
       <c r="BD4" s="12"/>
     </row>
     <row r="5" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>28</v>
-      </c>
+      <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
         <v>29</v>
       </c>
@@ -1560,10 +1554,10 @@
         <v>30</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>31</v>
@@ -1575,13 +1569,13 @@
         <v>17</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>19</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
@@ -1673,8 +1667,8 @@
   </sheetPr>
   <dimension ref="A1:XFD20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1783,7 +1777,7 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B4" s="22" t="s">
         <v>188</v>
@@ -1819,7 +1813,7 @@
     </row>
     <row r="5" s="3" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>190</v>
@@ -1867,7 +1861,7 @@
         <v>194</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="F6" s="22" t="s">
         <v>186</v>
@@ -1877,7 +1871,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="I6" s="22" t="n">
         <v>0.8</v>
@@ -1984,7 +1978,7 @@
     </row>
     <row r="4" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>37</v>
@@ -2020,7 +2014,7 @@
   </sheetPr>
   <dimension ref="A1:BM9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -2181,7 +2175,7 @@
         <v>53</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>51</v>
@@ -2280,10 +2274,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:T22"/>
+  <dimension ref="A1:XFD22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2407,6 +2401,9 @@
       <c r="R3" s="12"/>
       <c r="S3" s="12"/>
       <c r="T3" s="12"/>
+      <c r="XFB3" s="2"/>
+      <c r="XFC3" s="2"/>
+      <c r="XFD3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
@@ -2416,7 +2413,7 @@
         <v>74</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" s="19" t="s">
         <v>67</v>
@@ -2526,7 +2523,7 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2601,7 +2598,7 @@
         <v>0.9</v>
       </c>
       <c r="F3" s="19" t="n">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="12"/>
@@ -2688,8 +2685,8 @@
   </sheetPr>
   <dimension ref="A1:XFD26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2812,31 +2809,31 @@
         <v>105</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="I4" s="19" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J4" s="19" t="n">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="K4" s="19" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>75</v>
@@ -2845,16 +2842,16 @@
         <v>98</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F5" s="19" t="s">
         <v>100</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="I5" s="19" t="n">
         <v>8</v>
@@ -2869,10 +2866,10 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>75</v>
@@ -2881,16 +2878,16 @@
         <v>98</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>100</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="I6" s="19" t="n">
         <v>8</v>
@@ -2917,7 +2914,7 @@
         <v>98</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>100</v>
@@ -2953,25 +2950,25 @@
         <v>98</v>
       </c>
       <c r="E8" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="H8" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="G8" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>110</v>
-      </c>
       <c r="I8" s="19" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J8" s="19" t="n">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="K8" s="19" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="12"/>
@@ -2993,19 +2990,19 @@
         <v>125</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="G9" s="19" t="s">
         <v>101</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I9" s="19" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J9" s="19" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="K9" s="19" t="n">
         <v>3</v>
@@ -3127,7 +3124,7 @@
         <v>81</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>132</v>
@@ -3284,7 +3281,7 @@
   </sheetPr>
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>

</xml_diff>